<commit_message>
MTP052 COP rows provided
</commit_message>
<xml_diff>
--- a/observations/phobos_deimos/phobos_deimos.xlsx
+++ b/observations/phobos_deimos/phobos_deimos.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\phobos_deimos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CB322F6-1048-49BB-9DC5-5BB7D00CBBA0}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="10500"/>
+    <workbookView xWindow="3075" yWindow="3075" windowWidth="21600" windowHeight="11325" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
   <si>
     <t>PHOBOS DEIMOS COP ROWS</t>
   </si>
@@ -84,12 +85,15 @@
   </si>
   <si>
     <t>Meas Desc</t>
+  </si>
+  <si>
+    <t>LNO offset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -281,9 +285,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
@@ -307,12 +308,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -324,34 +319,43 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -633,11 +637,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -655,489 +659,561 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="B1" s="25"/>
+      <c r="C1" s="25"/>
+      <c r="L1" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
+      <c r="M1" s="25"/>
+      <c r="N1" s="25"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="3"/>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="12" t="s">
+      <c r="A3" s="2"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="14"/>
-      <c r="I3" s="15"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="23" t="s">
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="12"/>
+      <c r="L3" s="16"/>
+      <c r="M3" s="17"/>
+      <c r="N3" s="17"/>
+      <c r="O3" s="19" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="16" t="s">
+      <c r="A4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="17" t="s">
+      <c r="E4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="17" t="s">
+      <c r="F4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="I4" s="18" t="s">
+      <c r="I4" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="L4" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="M4" s="17" t="s">
+      <c r="M4" s="14" t="s">
         <v>18</v>
       </c>
-      <c r="N4" s="17" t="s">
+      <c r="N4" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="24" t="s">
+      <c r="O4" s="20" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="4">
         <v>51</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" s="5">
+      <c r="D5" s="4">
         <v>15</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>3</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G5" s="8">
+      <c r="G5" s="7">
         <v>16</v>
       </c>
-      <c r="H5" s="27">
+      <c r="H5" s="23">
         <v>3895</v>
       </c>
-      <c r="I5" s="28">
+      <c r="I5" s="24">
         <v>214</v>
       </c>
-      <c r="L5" s="5">
+      <c r="L5" s="4">
         <v>8</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>6</v>
       </c>
-      <c r="N5" s="6">
+      <c r="N5" s="5">
         <v>4</v>
       </c>
-      <c r="O5" s="25">
+      <c r="O5" s="21">
         <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>51</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="5">
+      <c r="D6" s="4">
         <v>15</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>3</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="G6" s="8">
+      <c r="G6" s="7">
         <v>16</v>
       </c>
-      <c r="H6" s="27">
+      <c r="H6" s="23">
         <v>3895</v>
       </c>
-      <c r="I6" s="28">
+      <c r="I6" s="24">
         <v>214</v>
       </c>
-      <c r="L6" s="5">
+      <c r="L6" s="4">
         <v>8</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>4</v>
       </c>
-      <c r="N6" s="6">
+      <c r="N6" s="5">
         <v>6</v>
       </c>
-      <c r="O6" s="25">
+      <c r="O6" s="21">
         <v>178</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="8"/>
-      <c r="L7" s="5">
+      <c r="A7" s="4">
+        <v>52</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" s="4">
+        <v>15</v>
+      </c>
+      <c r="E7" s="5">
+        <v>3</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="7">
+        <v>16</v>
+      </c>
+      <c r="H7" s="23">
+        <v>3895</v>
+      </c>
+      <c r="I7" s="24">
+        <v>214</v>
+      </c>
+      <c r="L7" s="4">
         <v>8</v>
       </c>
-      <c r="M7" s="22" t="s">
+      <c r="M7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="N7" s="6">
+      <c r="N7" s="5">
         <v>8</v>
       </c>
-      <c r="O7" s="25">
+      <c r="O7" s="21">
         <v>151</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="5"/>
-      <c r="B8" s="6"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="8"/>
-      <c r="L8" s="5">
+      <c r="A8" s="4">
+        <v>52</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="4">
+        <v>15</v>
+      </c>
+      <c r="E8" s="5">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="7">
+        <v>16</v>
+      </c>
+      <c r="H8" s="23">
+        <v>3895</v>
+      </c>
+      <c r="I8" s="24">
+        <v>214</v>
+      </c>
+      <c r="L8" s="4">
         <v>8</v>
       </c>
-      <c r="M8" s="22" t="s">
+      <c r="M8" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N8" s="6">
+      <c r="N8" s="5">
         <v>12</v>
       </c>
-      <c r="O8" s="25">
+      <c r="O8" s="21">
         <v>160</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="8"/>
-      <c r="L9" s="5">
+      <c r="A9" s="4">
+        <v>52</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D9" s="4">
+        <v>15</v>
+      </c>
+      <c r="E9" s="5">
+        <v>3</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="7">
+        <v>16</v>
+      </c>
+      <c r="H9" s="23">
+        <v>3895</v>
+      </c>
+      <c r="I9" s="24">
+        <v>214</v>
+      </c>
+      <c r="L9" s="4">
         <v>8</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <v>3</v>
       </c>
-      <c r="N9" s="6">
+      <c r="N9" s="5">
         <v>16</v>
       </c>
-      <c r="O9" s="25">
+      <c r="O9" s="21">
         <v>169</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A10" s="5"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="6"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="8"/>
-      <c r="L10" s="5"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="25"/>
+      <c r="A10" s="4">
+        <v>52</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D10" s="4">
+        <v>15</v>
+      </c>
+      <c r="E10" s="5">
+        <v>3</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="7">
+        <v>16</v>
+      </c>
+      <c r="H10" s="23">
+        <v>3895</v>
+      </c>
+      <c r="I10" s="24">
+        <v>214</v>
+      </c>
+      <c r="L10" s="4"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="21"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="8"/>
-      <c r="L11" s="5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="7"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="7"/>
+      <c r="L11" s="4">
         <v>15</v>
       </c>
-      <c r="M11" s="6">
+      <c r="M11" s="5">
         <v>6</v>
       </c>
-      <c r="N11" s="6">
+      <c r="N11" s="5">
         <v>4</v>
       </c>
-      <c r="O11" s="25">
+      <c r="O11" s="21">
         <v>187</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="5"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="8"/>
-      <c r="L12" s="5">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="4"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="7"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="7"/>
+      <c r="L12" s="4">
         <v>15</v>
       </c>
-      <c r="M12" s="6">
+      <c r="M12" s="5">
         <v>4</v>
       </c>
-      <c r="N12" s="6">
+      <c r="N12" s="5">
         <v>6</v>
       </c>
-      <c r="O12" s="25">
+      <c r="O12" s="21">
         <v>223</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="5"/>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="6"/>
-      <c r="F13" s="6"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="8"/>
-      <c r="L13" s="5">
+      <c r="A13" s="4"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="4"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="7"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="7"/>
+      <c r="L13" s="4">
         <v>15</v>
       </c>
-      <c r="M13" s="22" t="s">
+      <c r="M13" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="N13" s="6">
+      <c r="N13" s="5">
         <v>8</v>
       </c>
-      <c r="O13" s="25">
+      <c r="O13" s="21">
         <v>196</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="5"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="8"/>
-      <c r="L14" s="5">
+      <c r="A14" s="4"/>
+      <c r="B14" s="5"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="4"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="7"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="7"/>
+      <c r="L14" s="4">
         <v>15</v>
       </c>
-      <c r="M14" s="22" t="s">
+      <c r="M14" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="N14" s="6">
+      <c r="N14" s="5">
         <v>12</v>
       </c>
-      <c r="O14" s="25">
+      <c r="O14" s="21">
         <v>205</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="8"/>
-      <c r="L15" s="9">
+      <c r="A15" s="4"/>
+      <c r="B15" s="5"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="4"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="7"/>
+      <c r="L15" s="8">
         <v>15</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="9">
         <v>3</v>
       </c>
-      <c r="N15" s="10">
+      <c r="N15" s="9">
         <v>16</v>
       </c>
-      <c r="O15" s="26">
+      <c r="O15" s="22">
         <v>214</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="5"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="8"/>
+      <c r="A16" s="4"/>
+      <c r="B16" s="5"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="7"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="7"/>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A17" s="5"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="8"/>
+      <c r="A17" s="4"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="4"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="7"/>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A18" s="5"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="6"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="8"/>
+      <c r="A18" s="4"/>
+      <c r="B18" s="5"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="4"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="7"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="7"/>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="6"/>
-      <c r="F19" s="6"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="8"/>
+      <c r="A19" s="4"/>
+      <c r="B19" s="5"/>
+      <c r="C19" s="5"/>
+      <c r="D19" s="4"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="7"/>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="8"/>
+      <c r="A20" s="4"/>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="4"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="7"/>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="6"/>
-      <c r="F21" s="6"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="8"/>
+      <c r="A21" s="4"/>
+      <c r="B21" s="5"/>
+      <c r="C21" s="5"/>
+      <c r="D21" s="4"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="7"/>
+      <c r="H21" s="5"/>
+      <c r="I21" s="7"/>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="8"/>
+      <c r="A22" s="4"/>
+      <c r="B22" s="5"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="4"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="7"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="7"/>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
-      <c r="C23" s="6"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="6"/>
-      <c r="F23" s="6"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="8"/>
+      <c r="A23" s="4"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="4"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="5"/>
+      <c r="I23" s="7"/>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
-      <c r="C24" s="6"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="8"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="5"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="4"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="5"/>
+      <c r="I24" s="7"/>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
-      <c r="C25" s="6"/>
-      <c r="D25" s="5"/>
-      <c r="E25" s="6"/>
-      <c r="F25" s="6"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="6"/>
-      <c r="I25" s="8"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="5"/>
+      <c r="I25" s="7"/>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="6"/>
-      <c r="I26" s="8"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="5"/>
+      <c r="I26" s="7"/>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A27" s="9"/>
-      <c r="B27" s="10"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10"/>
-      <c r="F27" s="10"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="11"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="10"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="10"/>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>

</xml_diff>

<commit_message>
MTP068 done, kernel downloader updated
</commit_message>
<xml_diff>
--- a/observations/phobos_deimos/phobos_deimos.xlsx
+++ b/observations/phobos_deimos/phobos_deimos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\phobos_deimos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E514B308-6AAF-4172-84B4-96BA9AECAE26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D70DFA0-CC7D-4C88-B6C6-2D4A0323BB4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="139">
   <si>
     <t>PHOBOS DEIMOS COP ROWS</t>
   </si>
@@ -240,12 +240,6 @@
     <t>FULLSCAN 142 6 184 500MS</t>
   </si>
   <si>
-    <t>&lt;increase to 16 rows</t>
-  </si>
-  <si>
-    <t>&lt;60 seconds</t>
-  </si>
-  <si>
     <t>240,1,4081,4081,1,-1,PHOBOS,NONE,FULLSCAN ORDERS 6 142 184 WITH 16 ROWS 60S 500MS</t>
   </si>
   <si>
@@ -306,9 +300,6 @@
     <t>20221225_014801</t>
   </si>
   <si>
-    <t>2023-01-02T14:22:30</t>
-  </si>
-  <si>
     <t>20230104_051928</t>
   </si>
   <si>
@@ -330,27 +321,9 @@
     <t>2023-02-17T07:52:30</t>
   </si>
   <si>
-    <t>2023-02-28T18:59:30</t>
-  </si>
-  <si>
-    <t>2023-03-20T12:35:30</t>
-  </si>
-  <si>
-    <t>2023-03-23T01:30:30</t>
-  </si>
-  <si>
-    <t>2023-03-23T09:21:30</t>
-  </si>
-  <si>
-    <t>2022-12-31T03:24:30</t>
-  </si>
-  <si>
     <t>20230223_011421</t>
   </si>
   <si>
-    <t>2023 FEB 28 18:48:20</t>
-  </si>
-  <si>
     <t>20230127_113451</t>
   </si>
   <si>
@@ -370,13 +343,112 @@
   </si>
   <si>
     <t>20230225_220121</t>
+  </si>
+  <si>
+    <t>20230323_011917</t>
+  </si>
+  <si>
+    <t>20230323_091017</t>
+  </si>
+  <si>
+    <t>20230505_114846</t>
+  </si>
+  <si>
+    <t>20230511_131415</t>
+  </si>
+  <si>
+    <t>20230429_181516</t>
+  </si>
+  <si>
+    <t>20230320_122418</t>
+  </si>
+  <si>
+    <t>20230228_184820</t>
+  </si>
+  <si>
+    <t>&lt;-60 seconds</t>
+  </si>
+  <si>
+    <t>&lt;-increase to 16 rows</t>
+  </si>
+  <si>
+    <t>Not available, no TGO temperatures</t>
+  </si>
+  <si>
+    <t>20220909_032111</t>
+  </si>
+  <si>
+    <t>20220912_000810</t>
+  </si>
+  <si>
+    <t>20220914_205509</t>
+  </si>
+  <si>
+    <t>20220826_031920</t>
+  </si>
+  <si>
+    <t>20220826_190220</t>
+  </si>
+  <si>
+    <t>20220808_223604</t>
+  </si>
+  <si>
+    <t>20220823_063050</t>
+  </si>
+  <si>
+    <t>Green = available&gt;0.1a</t>
+  </si>
+  <si>
+    <t>20220719_102309</t>
+  </si>
+  <si>
+    <t>20220725_035605</t>
+  </si>
+  <si>
+    <t>20220714_004111</t>
+  </si>
+  <si>
+    <t>20220710_200313</t>
+  </si>
+  <si>
+    <t>20220713_164911</t>
+  </si>
+  <si>
+    <t>20220520_111259</t>
+  </si>
+  <si>
+    <t>20220523_000759</t>
+  </si>
+  <si>
+    <t>20220525_205458</t>
+  </si>
+  <si>
+    <t>20220526_044659</t>
+  </si>
+  <si>
+    <t>20220528_174158</t>
+  </si>
+  <si>
+    <t>20220531_142757</t>
+  </si>
+  <si>
+    <t>20230102_141059</t>
+  </si>
+  <si>
+    <t>20221231_031300</t>
+  </si>
+  <si>
+    <t>Orange = available@0.1a</t>
+  </si>
+  <si>
+    <t>Red = not available</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -421,8 +493,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -438,6 +524,16 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -619,11 +715,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -750,9 +848,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -760,9 +855,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -805,9 +897,37 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="13" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="12" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="11" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="3" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1088,54 +1208,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.88671875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5546875" customWidth="1"/>
-    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.88671875" style="47" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.44140625" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.140625" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5703125" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.42578125" style="47" customWidth="1"/>
+    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="41.44140625" customWidth="1"/>
+    <col min="18" max="18" width="41.42578125" customWidth="1"/>
     <col min="21" max="21" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="67" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="67"/>
-      <c r="C1" s="67"/>
-      <c r="M1" s="67" t="s">
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="M1" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="67"/>
-      <c r="O1" s="67"/>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="J2" s="80" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="68" t="s">
+      <c r="D3" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="69"/>
-      <c r="F3" s="69"/>
-      <c r="G3" s="70"/>
+      <c r="E3" s="67"/>
+      <c r="F3" s="67"/>
+      <c r="G3" s="68"/>
       <c r="H3" s="10"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="48"/>
+      <c r="J3" s="80" t="s">
+        <v>137</v>
+      </c>
       <c r="M3" s="15"/>
       <c r="N3" s="16"/>
       <c r="O3" s="16"/>
@@ -1143,7 +1270,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -1171,7 +1298,9 @@
       <c r="I4" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="49"/>
+      <c r="J4" s="48" t="s">
+        <v>123</v>
+      </c>
       <c r="M4" s="12" t="s">
         <v>7</v>
       </c>
@@ -1185,7 +1314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="15">
         <v>51</v>
       </c>
@@ -1201,19 +1330,21 @@
       <c r="E5" s="16">
         <v>3</v>
       </c>
-      <c r="F5" s="53" t="s">
+      <c r="F5" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="G5" s="54">
+      <c r="G5" s="52">
         <v>16</v>
       </c>
       <c r="H5" s="16">
         <v>3895</v>
       </c>
-      <c r="I5" s="55">
+      <c r="I5" s="53">
         <v>214</v>
       </c>
-      <c r="J5" s="56"/>
+      <c r="J5" s="76" t="s">
+        <v>129</v>
+      </c>
       <c r="M5" s="4">
         <v>8</v>
       </c>
@@ -1227,7 +1358,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="7">
         <v>51</v>
       </c>
@@ -1243,7 +1374,7 @@
       <c r="E6" s="8">
         <v>3</v>
       </c>
-      <c r="F6" s="57" t="s">
+      <c r="F6" s="55" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="9">
@@ -1252,10 +1383,12 @@
       <c r="H6" s="8">
         <v>3895</v>
       </c>
-      <c r="I6" s="58">
+      <c r="I6" s="56">
         <v>214</v>
       </c>
-      <c r="J6" s="51"/>
+      <c r="J6" s="71" t="s">
+        <v>130</v>
+      </c>
       <c r="M6" s="4">
         <v>8</v>
       </c>
@@ -1269,7 +1402,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>52</v>
       </c>
@@ -1297,7 +1430,9 @@
       <c r="I7" s="22">
         <v>214</v>
       </c>
-      <c r="J7" s="50"/>
+      <c r="J7" s="69" t="s">
+        <v>131</v>
+      </c>
       <c r="M7" s="4">
         <v>8</v>
       </c>
@@ -1311,7 +1446,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>52</v>
       </c>
@@ -1339,7 +1474,9 @@
       <c r="I8" s="22">
         <v>214</v>
       </c>
-      <c r="J8" s="50"/>
+      <c r="J8" s="69" t="s">
+        <v>132</v>
+      </c>
       <c r="M8" s="4">
         <v>8</v>
       </c>
@@ -1353,7 +1490,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>52</v>
       </c>
@@ -1381,7 +1518,9 @@
       <c r="I9" s="22">
         <v>214</v>
       </c>
-      <c r="J9" s="50"/>
+      <c r="J9" s="69" t="s">
+        <v>133</v>
+      </c>
       <c r="M9" s="4">
         <v>8</v>
       </c>
@@ -1395,7 +1534,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="7">
         <v>52</v>
       </c>
@@ -1411,7 +1550,7 @@
       <c r="E10" s="8">
         <v>3</v>
       </c>
-      <c r="F10" s="57" t="s">
+      <c r="F10" s="55" t="s">
         <v>54</v>
       </c>
       <c r="G10" s="9">
@@ -1420,16 +1559,18 @@
       <c r="H10" s="8">
         <v>3895</v>
       </c>
-      <c r="I10" s="58">
+      <c r="I10" s="56">
         <v>214</v>
       </c>
-      <c r="J10" s="51"/>
+      <c r="J10" s="71" t="s">
+        <v>134</v>
+      </c>
       <c r="M10" s="4"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="20"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>56</v>
       </c>
@@ -1457,7 +1598,9 @@
       <c r="I11" s="22">
         <v>205</v>
       </c>
-      <c r="J11" s="50"/>
+      <c r="J11" s="69" t="s">
+        <v>127</v>
+      </c>
       <c r="M11" s="4">
         <v>15</v>
       </c>
@@ -1471,7 +1614,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>56</v>
       </c>
@@ -1499,7 +1642,9 @@
       <c r="I12" s="22">
         <v>205</v>
       </c>
-      <c r="J12" s="50"/>
+      <c r="J12" s="69" t="s">
+        <v>128</v>
+      </c>
       <c r="M12" s="4">
         <v>15</v>
       </c>
@@ -1513,7 +1658,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>56</v>
       </c>
@@ -1541,7 +1686,9 @@
       <c r="I13" s="22">
         <v>205</v>
       </c>
-      <c r="J13" s="50"/>
+      <c r="J13" s="69" t="s">
+        <v>126</v>
+      </c>
       <c r="M13" s="4">
         <v>15</v>
       </c>
@@ -1555,7 +1702,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>56</v>
       </c>
@@ -1583,7 +1730,9 @@
       <c r="I14" s="22">
         <v>205</v>
       </c>
-      <c r="J14" s="50"/>
+      <c r="J14" s="69" t="s">
+        <v>124</v>
+      </c>
       <c r="M14" s="4">
         <v>15</v>
       </c>
@@ -1597,7 +1746,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>56</v>
       </c>
@@ -1613,7 +1762,7 @@
       <c r="E15" s="8">
         <v>6</v>
       </c>
-      <c r="F15" s="59" t="s">
+      <c r="F15" s="57" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="9">
@@ -1622,10 +1771,12 @@
       <c r="H15" s="8">
         <v>3893</v>
       </c>
-      <c r="I15" s="58">
+      <c r="I15" s="56">
         <v>205</v>
       </c>
-      <c r="J15" s="51"/>
+      <c r="J15" s="71" t="s">
+        <v>125</v>
+      </c>
       <c r="M15" s="7">
         <v>15</v>
       </c>
@@ -1639,7 +1790,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>57</v>
       </c>
@@ -1667,9 +1818,11 @@
       <c r="I16" s="22">
         <v>205</v>
       </c>
-      <c r="J16" s="50"/>
-    </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J16" s="69" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>57</v>
       </c>
@@ -1697,12 +1850,14 @@
       <c r="I17" s="22">
         <v>205</v>
       </c>
-      <c r="J17" s="50"/>
+      <c r="J17" s="69" t="s">
+        <v>122</v>
+      </c>
       <c r="N17" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>57</v>
       </c>
@@ -1730,9 +1885,11 @@
       <c r="I18" s="22">
         <v>205</v>
       </c>
-      <c r="J18" s="50"/>
-    </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J18" s="69" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>57</v>
       </c>
@@ -1748,7 +1905,7 @@
       <c r="E19" s="8">
         <v>6</v>
       </c>
-      <c r="F19" s="59" t="s">
+      <c r="F19" s="57" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="9">
@@ -1757,10 +1914,12 @@
       <c r="H19" s="8">
         <v>3893</v>
       </c>
-      <c r="I19" s="58">
+      <c r="I19" s="56">
         <v>205</v>
       </c>
-      <c r="J19" s="51"/>
+      <c r="J19" s="71" t="s">
+        <v>120</v>
+      </c>
       <c r="M19" s="15"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
@@ -1770,7 +1929,7 @@
       <c r="Q19" s="3"/>
       <c r="R19" s="26"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>58</v>
       </c>
@@ -1798,7 +1957,9 @@
       <c r="I20" s="22">
         <v>205</v>
       </c>
-      <c r="J20" s="50"/>
+      <c r="J20" s="69" t="s">
+        <v>116</v>
+      </c>
       <c r="M20" s="12" t="s">
         <v>7</v>
       </c>
@@ -1827,7 +1988,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>58</v>
       </c>
@@ -1855,7 +2016,9 @@
       <c r="I21" s="22">
         <v>205</v>
       </c>
-      <c r="J21" s="50"/>
+      <c r="J21" s="69" t="s">
+        <v>117</v>
+      </c>
       <c r="M21" s="15">
         <v>15</v>
       </c>
@@ -1882,7 +2045,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>58</v>
       </c>
@@ -1898,7 +2061,7 @@
       <c r="E22" s="8">
         <v>6</v>
       </c>
-      <c r="F22" s="60" t="s">
+      <c r="F22" s="58" t="s">
         <v>38</v>
       </c>
       <c r="G22" s="9">
@@ -1907,10 +2070,12 @@
       <c r="H22" s="8">
         <v>3799</v>
       </c>
-      <c r="I22" s="58">
+      <c r="I22" s="56">
         <v>205</v>
       </c>
-      <c r="J22" s="51"/>
+      <c r="J22" s="71" t="s">
+        <v>118</v>
+      </c>
       <c r="M22" s="4">
         <v>15</v>
       </c>
@@ -1940,7 +2105,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>59</v>
       </c>
@@ -1968,8 +2133,8 @@
       <c r="I23" s="22">
         <v>196</v>
       </c>
-      <c r="J23" s="50" t="s">
-        <v>79</v>
+      <c r="J23" s="79" t="s">
+        <v>77</v>
       </c>
       <c r="M23" s="4">
         <v>15</v>
@@ -2000,7 +2165,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>59</v>
       </c>
@@ -2028,8 +2193,8 @@
       <c r="I24" s="22">
         <v>205</v>
       </c>
-      <c r="J24" s="50" t="s">
-        <v>80</v>
+      <c r="J24" s="69" t="s">
+        <v>78</v>
       </c>
       <c r="M24" s="4">
         <v>15</v>
@@ -2060,7 +2225,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>59</v>
       </c>
@@ -2085,11 +2250,11 @@
       <c r="H25" s="8">
         <v>3813</v>
       </c>
-      <c r="I25" s="58">
+      <c r="I25" s="56">
         <v>205</v>
       </c>
-      <c r="J25" s="51" t="s">
-        <v>81</v>
+      <c r="J25" s="71" t="s">
+        <v>79</v>
       </c>
       <c r="M25" s="7">
         <v>15</v>
@@ -2120,7 +2285,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>60</v>
       </c>
@@ -2148,8 +2313,8 @@
       <c r="I26" s="22">
         <v>196</v>
       </c>
-      <c r="J26" s="50" t="s">
-        <v>82</v>
+      <c r="J26" s="69" t="s">
+        <v>80</v>
       </c>
       <c r="K26" t="s">
         <v>53</v>
@@ -2161,7 +2326,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="31"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>60</v>
       </c>
@@ -2189,8 +2354,8 @@
       <c r="I27" s="22">
         <v>196</v>
       </c>
-      <c r="J27" s="50" t="s">
-        <v>83</v>
+      <c r="J27" s="69" t="s">
+        <v>81</v>
       </c>
       <c r="M27" s="1"/>
       <c r="N27" s="1"/>
@@ -2199,7 +2364,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="31"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>60</v>
       </c>
@@ -2227,8 +2392,8 @@
       <c r="I28" s="22">
         <v>214</v>
       </c>
-      <c r="J28" s="50" t="s">
-        <v>84</v>
+      <c r="J28" s="69" t="s">
+        <v>82</v>
       </c>
       <c r="M28" s="1"/>
       <c r="N28" s="1"/>
@@ -2236,7 +2401,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>60</v>
       </c>
@@ -2252,7 +2417,7 @@
       <c r="E29" s="8">
         <v>3</v>
       </c>
-      <c r="F29" s="57" t="s">
+      <c r="F29" s="55" t="s">
         <v>54</v>
       </c>
       <c r="G29" s="9">
@@ -2261,11 +2426,11 @@
       <c r="H29" s="8">
         <v>3895</v>
       </c>
-      <c r="I29" s="58">
+      <c r="I29" s="56">
         <v>214</v>
       </c>
-      <c r="J29" s="51" t="s">
-        <v>85</v>
+      <c r="J29" s="71" t="s">
+        <v>83</v>
       </c>
       <c r="M29" s="1"/>
       <c r="N29" s="1"/>
@@ -2273,7 +2438,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A30" s="4">
         <v>61</v>
       </c>
@@ -2301,8 +2466,8 @@
       <c r="I30" s="22">
         <v>196</v>
       </c>
-      <c r="J30" s="50" t="s">
-        <v>86</v>
+      <c r="J30" s="69" t="s">
+        <v>84</v>
       </c>
       <c r="M30" s="1"/>
       <c r="N30" s="1"/>
@@ -2310,7 +2475,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A31" s="4">
         <v>61</v>
       </c>
@@ -2338,8 +2503,8 @@
       <c r="I31" s="22">
         <v>196</v>
       </c>
-      <c r="J31" s="50" t="s">
-        <v>87</v>
+      <c r="J31" s="69" t="s">
+        <v>85</v>
       </c>
       <c r="M31" s="1"/>
       <c r="N31" s="1"/>
@@ -2347,7 +2512,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A32" s="4">
         <v>61</v>
       </c>
@@ -2375,11 +2540,11 @@
       <c r="I32" s="22">
         <v>214</v>
       </c>
-      <c r="J32" s="50" t="s">
-        <v>88</v>
+      <c r="J32" s="69" t="s">
+        <v>86</v>
       </c>
       <c r="K32" t="s">
-        <v>71</v>
+        <v>114</v>
       </c>
       <c r="M32" s="1"/>
       <c r="N32" s="1"/>
@@ -2388,7 +2553,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="31"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A33" s="4">
         <v>61</v>
       </c>
@@ -2416,8 +2581,8 @@
       <c r="I33" s="22">
         <v>214</v>
       </c>
-      <c r="J33" s="50" t="s">
-        <v>89</v>
+      <c r="J33" s="69" t="s">
+        <v>87</v>
       </c>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
@@ -2425,7 +2590,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A34" s="4">
         <v>61</v>
       </c>
@@ -2453,8 +2618,8 @@
       <c r="I34" s="22">
         <v>214</v>
       </c>
-      <c r="J34" s="50" t="s">
-        <v>90</v>
+      <c r="J34" s="69" t="s">
+        <v>88</v>
       </c>
       <c r="M34" s="32" t="s">
         <v>47</v>
@@ -2465,7 +2630,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="31"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A35" s="7">
         <v>61</v>
       </c>
@@ -2481,7 +2646,7 @@
       <c r="E35" s="8">
         <v>3</v>
       </c>
-      <c r="F35" s="57" t="s">
+      <c r="F35" s="55" t="s">
         <v>54</v>
       </c>
       <c r="G35" s="9">
@@ -2490,11 +2655,11 @@
       <c r="H35" s="8">
         <v>3895</v>
       </c>
-      <c r="I35" s="58">
+      <c r="I35" s="56">
         <v>214</v>
       </c>
-      <c r="J35" s="51" t="s">
-        <v>91</v>
+      <c r="J35" s="71" t="s">
+        <v>89</v>
       </c>
       <c r="M35" s="1"/>
       <c r="N35" s="1"/>
@@ -2503,7 +2668,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="31"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A36" s="4">
         <v>62</v>
       </c>
@@ -2531,16 +2696,16 @@
       <c r="I36" s="22">
         <v>214</v>
       </c>
-      <c r="J36" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="M36" s="67" t="s">
+      <c r="J36" s="69" t="s">
+        <v>90</v>
+      </c>
+      <c r="M36" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="N36" s="67"/>
-      <c r="O36" s="67"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="N36" s="65"/>
+      <c r="O36" s="65"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>62</v>
       </c>
@@ -2568,11 +2733,11 @@
       <c r="I37" s="22">
         <v>214</v>
       </c>
-      <c r="J37" s="52" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J37" s="69" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A38" s="4">
         <v>62</v>
       </c>
@@ -2600,8 +2765,8 @@
       <c r="I38" s="22">
         <v>214</v>
       </c>
-      <c r="J38" s="50" t="s">
-        <v>93</v>
+      <c r="J38" s="69" t="s">
+        <v>135</v>
       </c>
       <c r="M38" s="15"/>
       <c r="N38" s="16"/>
@@ -2610,7 +2775,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A39" s="4">
         <v>62</v>
       </c>
@@ -2638,8 +2803,8 @@
       <c r="I39" s="22">
         <v>214</v>
       </c>
-      <c r="J39" s="50" t="s">
-        <v>94</v>
+      <c r="J39" s="69" t="s">
+        <v>91</v>
       </c>
       <c r="M39" s="12" t="s">
         <v>7</v>
@@ -2654,7 +2819,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A40" s="4">
         <v>62</v>
       </c>
@@ -2682,8 +2847,8 @@
       <c r="I40" s="22">
         <v>214</v>
       </c>
-      <c r="J40" s="50" t="s">
-        <v>95</v>
+      <c r="J40" s="69" t="s">
+        <v>92</v>
       </c>
       <c r="M40" s="4">
         <v>15</v>
@@ -2698,7 +2863,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A41" s="4">
         <v>62</v>
       </c>
@@ -2726,8 +2891,8 @@
       <c r="I41" s="22">
         <v>214</v>
       </c>
-      <c r="J41" s="50" t="s">
-        <v>96</v>
+      <c r="J41" s="69" t="s">
+        <v>93</v>
       </c>
       <c r="M41" s="4">
         <v>15</v>
@@ -2742,7 +2907,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A42" s="7">
         <v>62</v>
       </c>
@@ -2758,7 +2923,7 @@
       <c r="E42" s="8">
         <v>3</v>
       </c>
-      <c r="F42" s="57" t="s">
+      <c r="F42" s="55" t="s">
         <v>54</v>
       </c>
       <c r="G42" s="9">
@@ -2767,11 +2932,11 @@
       <c r="H42" s="8">
         <v>3895</v>
       </c>
-      <c r="I42" s="58">
+      <c r="I42" s="56">
         <v>214</v>
       </c>
-      <c r="J42" s="51" t="s">
-        <v>97</v>
+      <c r="J42" s="71" t="s">
+        <v>94</v>
       </c>
       <c r="M42" s="33">
         <v>15</v>
@@ -2786,7 +2951,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A43" s="4">
         <v>63</v>
       </c>
@@ -2814,8 +2979,8 @@
       <c r="I43" s="22">
         <v>214</v>
       </c>
-      <c r="J43" s="50" t="s">
-        <v>108</v>
+      <c r="J43" s="79" t="s">
+        <v>99</v>
       </c>
       <c r="M43" s="37">
         <v>15</v>
@@ -2830,7 +2995,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A44" s="4">
         <v>63</v>
       </c>
@@ -2858,11 +3023,11 @@
       <c r="I44" s="22">
         <v>214</v>
       </c>
-      <c r="J44" s="50" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J44" s="69" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A45" s="4">
         <v>63</v>
       </c>
@@ -2890,14 +3055,14 @@
       <c r="I45" s="22">
         <v>214</v>
       </c>
-      <c r="J45" s="50" t="s">
-        <v>99</v>
+      <c r="J45" s="69" t="s">
+        <v>96</v>
       </c>
       <c r="N45" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A46" s="7">
         <v>63</v>
       </c>
@@ -2922,14 +3087,17 @@
       <c r="H46" s="8">
         <v>423</v>
       </c>
-      <c r="I46" s="58">
+      <c r="I46" s="56">
         <v>214</v>
       </c>
-      <c r="J46" s="51" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="J46" s="78" t="s">
+        <v>97</v>
+      </c>
+      <c r="K46" s="77" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A47" s="4">
         <v>64</v>
       </c>
@@ -2939,16 +3107,16 @@
       <c r="C47" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D47" s="4">
+      <c r="D47" s="15">
         <v>60</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E47" s="16">
         <v>3</v>
       </c>
-      <c r="F47" s="1" t="s">
+      <c r="F47" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="G47" s="6">
+      <c r="G47" s="52">
         <v>16</v>
       </c>
       <c r="H47" s="1">
@@ -2957,11 +3125,11 @@
       <c r="I47" s="6">
         <v>240</v>
       </c>
-      <c r="J47" s="50" t="s">
-        <v>106</v>
+      <c r="J47" s="79" t="s">
+        <v>98</v>
       </c>
       <c r="K47" t="s">
-        <v>72</v>
+        <v>113</v>
       </c>
       <c r="M47" s="15"/>
       <c r="N47" s="16"/>
@@ -2972,7 +3140,7 @@
       <c r="Q47" s="3"/>
       <c r="R47" s="26"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A48" s="4">
         <v>64</v>
       </c>
@@ -2985,10 +3153,10 @@
       <c r="D48" s="4">
         <v>60</v>
       </c>
-      <c r="E48" s="1">
+      <c r="E48" s="74">
         <v>3</v>
       </c>
-      <c r="F48" s="1" t="s">
+      <c r="F48" s="74" t="s">
         <v>70</v>
       </c>
       <c r="G48" s="6">
@@ -3000,8 +3168,8 @@
       <c r="I48" s="6">
         <v>240</v>
       </c>
-      <c r="J48" s="50" t="s">
-        <v>114</v>
+      <c r="J48" s="79" t="s">
+        <v>105</v>
       </c>
       <c r="M48" s="12" t="s">
         <v>7</v>
@@ -3031,7 +3199,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A49" s="7">
         <v>64</v>
       </c>
@@ -3047,8 +3215,8 @@
       <c r="E49" s="8">
         <v>3</v>
       </c>
-      <c r="F49" s="57" t="s">
-        <v>54</v>
+      <c r="F49" s="55" t="s">
+        <v>58</v>
       </c>
       <c r="G49" s="9">
         <v>16</v>
@@ -3056,14 +3224,11 @@
       <c r="H49" s="8">
         <v>3895</v>
       </c>
-      <c r="I49" s="58">
+      <c r="I49" s="56">
         <v>214</v>
       </c>
-      <c r="J49" s="51" t="s">
-        <v>101</v>
-      </c>
-      <c r="K49" t="s">
-        <v>107</v>
+      <c r="J49" s="71" t="s">
+        <v>112</v>
       </c>
       <c r="M49" s="15">
         <v>15</v>
@@ -3091,7 +3256,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A50" s="4">
         <v>65</v>
       </c>
@@ -3099,7 +3264,7 @@
         <v>5</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D50" s="4">
         <v>60</v>
@@ -3108,7 +3273,7 @@
         <v>6</v>
       </c>
       <c r="F50" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G50" s="6">
         <v>12</v>
@@ -3119,8 +3284,8 @@
       <c r="I50" s="6">
         <v>235</v>
       </c>
-      <c r="J50" s="50" t="s">
-        <v>102</v>
+      <c r="J50" s="69" t="s">
+        <v>111</v>
       </c>
       <c r="M50" s="4">
         <v>15</v>
@@ -3148,7 +3313,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A51" s="4">
         <v>65</v>
       </c>
@@ -3156,7 +3321,7 @@
         <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D51" s="4">
         <v>60</v>
@@ -3165,7 +3330,7 @@
         <v>6</v>
       </c>
       <c r="F51" s="44" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G51" s="6">
         <v>12</v>
@@ -3176,8 +3341,8 @@
       <c r="I51" s="6">
         <v>235</v>
       </c>
-      <c r="J51" s="50" t="s">
-        <v>103</v>
+      <c r="J51" s="69" t="s">
+        <v>106</v>
       </c>
       <c r="M51" s="4">
         <v>15</v>
@@ -3205,7 +3370,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="7">
         <v>65</v>
       </c>
@@ -3213,7 +3378,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D52" s="7">
         <v>60</v>
@@ -3221,8 +3386,8 @@
       <c r="E52" s="8">
         <v>6</v>
       </c>
-      <c r="F52" s="61" t="s">
-        <v>78</v>
+      <c r="F52" s="59" t="s">
+        <v>76</v>
       </c>
       <c r="G52" s="9">
         <v>12</v>
@@ -3233,8 +3398,8 @@
       <c r="I52" s="9">
         <v>235</v>
       </c>
-      <c r="J52" s="51" t="s">
-        <v>104</v>
+      <c r="J52" s="71" t="s">
+        <v>107</v>
       </c>
       <c r="M52" s="4">
         <v>15</v>
@@ -3262,7 +3427,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A53" s="4">
         <v>66</v>
       </c>
@@ -3270,7 +3435,7 @@
         <v>5</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D53" s="4">
         <v>60</v>
@@ -3279,7 +3444,7 @@
         <v>6</v>
       </c>
       <c r="F53" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="G53" s="6">
         <v>12</v>
@@ -3290,7 +3455,9 @@
       <c r="I53" s="6">
         <v>235</v>
       </c>
-      <c r="J53" s="56"/>
+      <c r="J53" s="70" t="s">
+        <v>110</v>
+      </c>
       <c r="M53" s="37">
         <v>15</v>
       </c>
@@ -3317,7 +3484,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A54" s="4">
         <v>66</v>
       </c>
@@ -3325,7 +3492,7 @@
         <v>5</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D54" s="4">
         <v>60</v>
@@ -3334,7 +3501,7 @@
         <v>6</v>
       </c>
       <c r="F54" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="G54" s="6">
         <v>12</v>
@@ -3345,9 +3512,11 @@
       <c r="I54" s="6">
         <v>235</v>
       </c>
-      <c r="J54" s="50"/>
-    </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J54" s="72" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A55" s="7">
         <v>66</v>
       </c>
@@ -3355,7 +3524,7 @@
         <v>5</v>
       </c>
       <c r="C55" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D55" s="7">
         <v>60</v>
@@ -3363,8 +3532,8 @@
       <c r="E55" s="8">
         <v>6</v>
       </c>
-      <c r="F55" s="60" t="s">
-        <v>113</v>
+      <c r="F55" s="58" t="s">
+        <v>104</v>
       </c>
       <c r="G55" s="9">
         <v>12</v>
@@ -3375,36 +3544,74 @@
       <c r="I55" s="9">
         <v>235</v>
       </c>
-      <c r="J55" s="51"/>
-    </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A56" s="4">
-        <v>67</v>
-      </c>
-      <c r="B56" s="1"/>
-      <c r="C56" s="1"/>
-      <c r="D56" s="4"/>
-      <c r="E56" s="1"/>
-      <c r="F56" s="1"/>
-      <c r="G56" s="6"/>
-      <c r="H56" s="1"/>
-      <c r="I56" s="6"/>
-      <c r="J56" s="50"/>
-    </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A57" s="4"/>
-      <c r="B57" s="1"/>
-      <c r="C57" s="1"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="1"/>
-      <c r="F57" s="1"/>
-      <c r="G57" s="6"/>
-      <c r="H57" s="1"/>
-      <c r="I57" s="6"/>
+      <c r="J55" s="73" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A56" s="15">
+        <v>68</v>
+      </c>
+      <c r="B56" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C56" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="D56" s="15">
+        <v>60</v>
+      </c>
+      <c r="E56" s="16">
+        <v>6</v>
+      </c>
+      <c r="F56" s="75" t="s">
+        <v>76</v>
+      </c>
+      <c r="G56" s="52">
+        <v>12</v>
+      </c>
+      <c r="H56" s="16">
+        <v>3992</v>
+      </c>
+      <c r="I56" s="52">
+        <v>235</v>
+      </c>
+      <c r="J56" s="54"/>
+    </row>
+    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A57" s="7">
+        <v>68</v>
+      </c>
+      <c r="B57" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C57" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D57" s="7">
+        <v>60</v>
+      </c>
+      <c r="E57" s="8">
+        <v>6</v>
+      </c>
+      <c r="F57" s="59" t="s">
+        <v>76</v>
+      </c>
+      <c r="G57" s="9">
+        <v>12</v>
+      </c>
+      <c r="H57" s="8">
+        <v>3992</v>
+      </c>
+      <c r="I57" s="9">
+        <v>235</v>
+      </c>
       <c r="J57" s="50"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="A58" s="4"/>
+    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A58" s="4">
+        <v>69</v>
+      </c>
       <c r="B58" s="1"/>
       <c r="C58" s="1"/>
       <c r="D58" s="4"/>
@@ -3413,9 +3620,9 @@
       <c r="G58" s="6"/>
       <c r="H58" s="1"/>
       <c r="I58" s="6"/>
-      <c r="J58" s="50"/>
-    </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J58" s="49"/>
+    </row>
+    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A59" s="4"/>
       <c r="B59" s="1"/>
       <c r="C59" s="1"/>
@@ -3425,9 +3632,9 @@
       <c r="G59" s="6"/>
       <c r="H59" s="1"/>
       <c r="I59" s="6"/>
-      <c r="J59" s="50"/>
-    </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J59" s="49"/>
+    </row>
+    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A60" s="4"/>
       <c r="B60" s="1"/>
       <c r="C60" s="1"/>
@@ -3437,12 +3644,12 @@
       <c r="G60" s="6"/>
       <c r="H60" s="1"/>
       <c r="I60" s="6"/>
-      <c r="J60" s="50"/>
+      <c r="J60" s="49"/>
       <c r="M60" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A61" s="4"/>
       <c r="B61" s="1"/>
       <c r="C61" s="1"/>
@@ -3452,9 +3659,9 @@
       <c r="G61" s="6"/>
       <c r="H61" s="1"/>
       <c r="I61" s="6"/>
-      <c r="J61" s="50"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J61" s="49"/>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A62" s="4"/>
       <c r="B62" s="1"/>
       <c r="C62" s="1"/>
@@ -3464,14 +3671,14 @@
       <c r="G62" s="6"/>
       <c r="H62" s="1"/>
       <c r="I62" s="6"/>
-      <c r="J62" s="50"/>
-      <c r="N62" s="67" t="s">
+      <c r="J62" s="49"/>
+      <c r="N62" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="O62" s="67"/>
-      <c r="P62" s="67"/>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="O62" s="65"/>
+      <c r="P62" s="65"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A63" s="4"/>
       <c r="B63" s="1"/>
       <c r="C63" s="1"/>
@@ -3481,9 +3688,9 @@
       <c r="G63" s="6"/>
       <c r="H63" s="1"/>
       <c r="I63" s="6"/>
-      <c r="J63" s="50"/>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="J63" s="49"/>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A64" s="4"/>
       <c r="B64" s="1"/>
       <c r="C64" s="1"/>
@@ -3493,7 +3700,7 @@
       <c r="G64" s="6"/>
       <c r="H64" s="1"/>
       <c r="I64" s="6"/>
-      <c r="J64" s="50"/>
+      <c r="J64" s="49"/>
       <c r="M64" s="15"/>
       <c r="N64" s="16"/>
       <c r="O64" s="16"/>
@@ -3501,7 +3708,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A65" s="4"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3511,7 +3718,7 @@
       <c r="G65" s="6"/>
       <c r="H65" s="1"/>
       <c r="I65" s="6"/>
-      <c r="J65" s="50"/>
+      <c r="J65" s="49"/>
       <c r="M65" s="12" t="s">
         <v>7</v>
       </c>
@@ -3525,7 +3732,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3535,7 +3742,7 @@
       <c r="G66" s="6"/>
       <c r="H66" s="1"/>
       <c r="I66" s="6"/>
-      <c r="J66" s="50"/>
+      <c r="J66" s="49"/>
       <c r="M66" s="41">
         <v>15</v>
       </c>
@@ -3549,7 +3756,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A67" s="4"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3559,7 +3766,7 @@
       <c r="G67" s="6"/>
       <c r="H67" s="1"/>
       <c r="I67" s="6"/>
-      <c r="J67" s="50"/>
+      <c r="J67" s="49"/>
       <c r="M67">
         <v>30</v>
       </c>
@@ -3573,7 +3780,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -3583,7 +3790,7 @@
       <c r="G68" s="9"/>
       <c r="H68" s="8"/>
       <c r="I68" s="9"/>
-      <c r="J68" s="51"/>
+      <c r="J68" s="50"/>
       <c r="M68">
         <v>60</v>
       </c>
@@ -3597,7 +3804,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3620,7 +3827,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3634,7 +3841,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3645,7 +3852,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M72" s="15"/>
       <c r="N72" s="16"/>
       <c r="O72" s="16"/>
@@ -3655,7 +3862,7 @@
       <c r="Q72" s="3"/>
       <c r="R72" s="26"/>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M73" s="12" t="s">
         <v>7</v>
       </c>
@@ -3684,7 +3891,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M74" s="15">
         <v>15</v>
       </c>
@@ -3714,7 +3921,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M75" s="1">
         <v>15</v>
       </c>
@@ -3741,7 +3948,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
       <c r="M76" s="41">
         <v>15</v>
       </c>
@@ -3768,11 +3975,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="13:22" x14ac:dyDescent="0.3">
-      <c r="M81" s="65"/>
+    <row r="81" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="M81" s="63"/>
       <c r="N81" s="10"/>
       <c r="O81" s="10"/>
-      <c r="P81" s="66" t="s">
+      <c r="P81" s="64" t="s">
         <v>66</v>
       </c>
       <c r="Q81" s="10" t="s">
@@ -3780,8 +3987,8 @@
       </c>
       <c r="R81" s="11"/>
     </row>
-    <row r="82" spans="13:22" x14ac:dyDescent="0.3">
-      <c r="M82" s="62">
+    <row r="82" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="M82" s="60">
         <v>60</v>
       </c>
       <c r="N82">
@@ -3807,11 +4014,11 @@
         <v>67</v>
       </c>
       <c r="V82" s="31" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="83" spans="13:22" x14ac:dyDescent="0.3">
-      <c r="M83" s="62">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="83" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="M83" s="60">
         <v>60</v>
       </c>
       <c r="N83">
@@ -3837,11 +4044,11 @@
         <v>67</v>
       </c>
       <c r="V83" s="31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="84" spans="13:22" x14ac:dyDescent="0.3">
-      <c r="M84" s="62">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="84" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="M84" s="60">
         <v>60</v>
       </c>
       <c r="N84">
@@ -3857,18 +4064,18 @@
         <v>235</v>
       </c>
       <c r="R84" s="27" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="T84">
         <f t="shared" ref="T84:T86" si="0">P84+2</f>
         <v>3994</v>
       </c>
       <c r="U84" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="85" spans="13:22" x14ac:dyDescent="0.3">
-      <c r="M85" s="62">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="85" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="M85" s="60">
         <v>60</v>
       </c>
       <c r="N85">
@@ -3884,41 +4091,41 @@
         <v>235</v>
       </c>
       <c r="R85" s="27" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="T85">
         <f t="shared" si="0"/>
         <v>3924</v>
       </c>
       <c r="U85" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="86" spans="13:22" x14ac:dyDescent="0.3">
-      <c r="M86" s="63">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="86" spans="13:22" x14ac:dyDescent="0.25">
+      <c r="M86" s="61">
         <v>60</v>
       </c>
-      <c r="N86" s="60">
+      <c r="N86" s="58">
         <v>6</v>
       </c>
-      <c r="O86" s="60">
+      <c r="O86" s="58">
         <v>12</v>
       </c>
-      <c r="P86" s="64">
+      <c r="P86" s="62">
         <v>3914</v>
       </c>
-      <c r="Q86" s="60">
+      <c r="Q86" s="58">
         <v>235</v>
       </c>
       <c r="R86" s="29" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="T86">
         <f t="shared" si="0"/>
         <v>3916</v>
       </c>
       <c r="U86" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
     </row>
   </sheetData>
@@ -3930,7 +4137,7 @@
     <mergeCell ref="N62:P62"/>
   </mergeCells>
   <conditionalFormatting sqref="H5">
-    <cfRule type="iconSet" priority="96">
+    <cfRule type="iconSet" priority="98">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -3938,7 +4145,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="97">
+    <cfRule type="iconSet" priority="99">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -3948,7 +4155,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5">
-    <cfRule type="colorScale" priority="93">
+    <cfRule type="colorScale" priority="95">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3956,7 +4163,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="95">
+    <cfRule type="colorScale" priority="97">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3968,7 +4175,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:J9">
-    <cfRule type="colorScale" priority="57">
+    <cfRule type="colorScale" priority="59">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -3976,7 +4183,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="58">
+    <cfRule type="colorScale" priority="60">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -3988,7 +4195,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H30 H32:H35">
-    <cfRule type="iconSet" priority="55">
+    <cfRule type="iconSet" priority="57">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -3996,7 +4203,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="56">
+    <cfRule type="iconSet" priority="58">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4006,7 +4213,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="iconSet" priority="51">
+    <cfRule type="iconSet" priority="53">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4014,7 +4221,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="52">
+    <cfRule type="iconSet" priority="54">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4024,7 +4231,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:J22 I24:J35 I23 J16:J31">
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4032,7 +4239,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="50">
+    <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4043,8 +4250,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I5:J22 I47:J48 I24:J35 I23 J16:J31 I50:J54">
-    <cfRule type="colorScale" priority="47">
+  <conditionalFormatting sqref="I5:J22 I47:J48 I24:J35 I23 J16:J31 I50:J52 I53:I54">
+    <cfRule type="colorScale" priority="49">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4056,7 +4263,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:H37">
-    <cfRule type="iconSet" priority="45">
+    <cfRule type="iconSet" priority="47">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4064,7 +4271,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="46">
+    <cfRule type="iconSet" priority="48">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4074,7 +4281,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:J37">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4082,7 +4289,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4094,7 +4301,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:J37">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="44">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4106,7 +4313,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:H39">
-    <cfRule type="iconSet" priority="40">
+    <cfRule type="iconSet" priority="42">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4114,7 +4321,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="41">
+    <cfRule type="iconSet" priority="43">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4124,7 +4331,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:J39">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4132,7 +4339,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4144,7 +4351,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:J39">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4156,7 +4363,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="iconSet" priority="35">
+    <cfRule type="iconSet" priority="37">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4164,7 +4371,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="36">
+    <cfRule type="iconSet" priority="38">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4174,7 +4381,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:J40">
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4182,7 +4389,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4194,7 +4401,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:J40">
-    <cfRule type="colorScale" priority="32">
+    <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4206,7 +4413,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41:H42">
-    <cfRule type="iconSet" priority="30">
+    <cfRule type="iconSet" priority="32">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4214,7 +4421,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="31">
+    <cfRule type="iconSet" priority="33">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4224,7 +4431,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:J42">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4232,7 +4439,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4244,7 +4451,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:J42">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="29">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4256,7 +4463,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="iconSet" priority="25">
+    <cfRule type="iconSet" priority="27">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4264,7 +4471,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="26">
+    <cfRule type="iconSet" priority="28">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4274,7 +4481,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:J43">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4282,7 +4489,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4294,7 +4501,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:J43">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="24">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4306,7 +4513,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="iconSet" priority="20">
+    <cfRule type="iconSet" priority="22">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4314,7 +4521,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="21">
+    <cfRule type="iconSet" priority="23">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4324,7 +4531,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44:J44">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4332,7 +4539,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4344,7 +4551,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44:J44">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4356,7 +4563,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="iconSet" priority="15">
+    <cfRule type="iconSet" priority="17">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4364,7 +4571,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="16">
+    <cfRule type="iconSet" priority="18">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4374,7 +4581,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:J45">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4382,7 +4589,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4394,7 +4601,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:J45">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4406,7 +4613,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="iconSet" priority="10">
+    <cfRule type="iconSet" priority="12">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4414,7 +4621,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="11">
+    <cfRule type="iconSet" priority="13">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4424,7 +4631,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46:J46">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="10">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4432,7 +4639,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4444,7 +4651,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46:J46">
-    <cfRule type="colorScale" priority="7">
+    <cfRule type="colorScale" priority="9">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4456,7 +4663,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="iconSet" priority="5">
+    <cfRule type="iconSet" priority="7">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4464,7 +4671,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="6">
+    <cfRule type="iconSet" priority="8">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4474,7 +4681,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:J49">
-    <cfRule type="colorScale" priority="3">
+    <cfRule type="colorScale" priority="5">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4482,7 +4689,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="4">
+    <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4494,6 +4701,30 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:J49">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I55">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I56">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -4505,7 +4736,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I55">
+  <conditionalFormatting sqref="I57">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
LNO phobos spreadsheet updated
</commit_message>
<xml_diff>
--- a/observations/phobos_deimos/phobos_deimos.xlsx
+++ b/observations/phobos_deimos/phobos_deimos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\phobos_deimos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F49F89-E2DC-48B2-BAF1-08845E098960}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF586435-7257-4882-92CC-994F95179D04}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="154">
   <si>
     <t>PHOBOS DEIMOS COP ROWS</t>
   </si>
@@ -462,16 +462,31 @@
     <t>GAP 3 ORDERS 157 160 163 166 169 172 500MS</t>
   </si>
   <si>
-    <t>2023-07-13T09:39:30</t>
-  </si>
-  <si>
-    <t>2023-07-16T06:26:00</t>
-  </si>
-  <si>
-    <t>2023-07-01T22:31:30</t>
-  </si>
-  <si>
-    <t>2023-07-03T19:43:30</t>
+    <t>20230713_092806</t>
+  </si>
+  <si>
+    <t>20230716_061435</t>
+  </si>
+  <si>
+    <t>20230701_222009</t>
+  </si>
+  <si>
+    <t>20230703_193210</t>
+  </si>
+  <si>
+    <t>2023-10-24T11:43:30</t>
+  </si>
+  <si>
+    <t>2023-10-27T08:30:15</t>
+  </si>
+  <si>
+    <t>2023-09-03T02:37:30</t>
+  </si>
+  <si>
+    <t>2023-08-28T01:12:00</t>
+  </si>
+  <si>
+    <t>2023-08-30T06:15:30</t>
   </si>
 </sst>
 </file>
@@ -751,7 +766,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="78">
+  <cellXfs count="81">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -895,9 +910,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -947,6 +959,18 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1233,59 +1257,59 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
-      <selection activeCell="H63" sqref="H63"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G64" sqref="G64:G65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="44.85546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.5703125" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="23.42578125" style="47" customWidth="1"/>
-    <col min="15" max="15" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" customWidth="1"/>
+    <col min="1" max="1" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.88671875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="44.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.5546875" customWidth="1"/>
+    <col min="8" max="8" width="16.109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23.44140625" style="47" customWidth="1"/>
+    <col min="15" max="15" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.44140625" customWidth="1"/>
     <col min="17" max="17" width="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="41.42578125" customWidth="1"/>
+    <col min="18" max="18" width="41.44140625" customWidth="1"/>
     <col min="21" max="21" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A1" s="74" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A1" s="73" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="74"/>
-      <c r="C1" s="74"/>
-      <c r="M1" s="74" t="s">
+      <c r="B1" s="73"/>
+      <c r="C1" s="73"/>
+      <c r="M1" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="74"/>
-      <c r="O1" s="74"/>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="J2" s="73" t="s">
+      <c r="N1" s="73"/>
+      <c r="O1" s="73"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="J2" s="72" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="75" t="s">
+      <c r="D3" s="74" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="76"/>
-      <c r="F3" s="76"/>
-      <c r="G3" s="77"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="75"/>
+      <c r="G3" s="76"/>
       <c r="H3" s="10"/>
       <c r="I3" s="11"/>
-      <c r="J3" s="73" t="s">
+      <c r="J3" s="72" t="s">
         <v>137</v>
       </c>
       <c r="M3" s="15"/>
@@ -1295,7 +1319,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A4" s="12" t="s">
         <v>2</v>
       </c>
@@ -1339,7 +1363,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A5" s="15">
         <v>51</v>
       </c>
@@ -1367,7 +1391,7 @@
       <c r="I5" s="53">
         <v>214</v>
       </c>
-      <c r="J5" s="69" t="s">
+      <c r="J5" s="68" t="s">
         <v>129</v>
       </c>
       <c r="M5" s="4">
@@ -1383,7 +1407,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A6" s="7">
         <v>51</v>
       </c>
@@ -1399,7 +1423,7 @@
       <c r="E6" s="8">
         <v>3</v>
       </c>
-      <c r="F6" s="55" t="s">
+      <c r="F6" s="54" t="s">
         <v>54</v>
       </c>
       <c r="G6" s="9">
@@ -1408,10 +1432,10 @@
       <c r="H6" s="8">
         <v>3895</v>
       </c>
-      <c r="I6" s="56">
+      <c r="I6" s="55">
         <v>214</v>
       </c>
-      <c r="J6" s="66" t="s">
+      <c r="J6" s="65" t="s">
         <v>130</v>
       </c>
       <c r="M6" s="4">
@@ -1427,7 +1451,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A7" s="4">
         <v>52</v>
       </c>
@@ -1455,7 +1479,7 @@
       <c r="I7" s="22">
         <v>214</v>
       </c>
-      <c r="J7" s="64" t="s">
+      <c r="J7" s="63" t="s">
         <v>131</v>
       </c>
       <c r="M7" s="4">
@@ -1471,7 +1495,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A8" s="4">
         <v>52</v>
       </c>
@@ -1499,7 +1523,7 @@
       <c r="I8" s="22">
         <v>214</v>
       </c>
-      <c r="J8" s="64" t="s">
+      <c r="J8" s="63" t="s">
         <v>132</v>
       </c>
       <c r="M8" s="4">
@@ -1515,7 +1539,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A9" s="4">
         <v>52</v>
       </c>
@@ -1543,7 +1567,7 @@
       <c r="I9" s="22">
         <v>214</v>
       </c>
-      <c r="J9" s="64" t="s">
+      <c r="J9" s="63" t="s">
         <v>133</v>
       </c>
       <c r="M9" s="4">
@@ -1559,7 +1583,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A10" s="7">
         <v>52</v>
       </c>
@@ -1575,7 +1599,7 @@
       <c r="E10" s="8">
         <v>3</v>
       </c>
-      <c r="F10" s="55" t="s">
+      <c r="F10" s="54" t="s">
         <v>54</v>
       </c>
       <c r="G10" s="9">
@@ -1584,10 +1608,10 @@
       <c r="H10" s="8">
         <v>3895</v>
       </c>
-      <c r="I10" s="56">
+      <c r="I10" s="55">
         <v>214</v>
       </c>
-      <c r="J10" s="66" t="s">
+      <c r="J10" s="65" t="s">
         <v>134</v>
       </c>
       <c r="M10" s="4"/>
@@ -1595,7 +1619,7 @@
       <c r="O10" s="1"/>
       <c r="P10" s="20"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
         <v>56</v>
       </c>
@@ -1623,7 +1647,7 @@
       <c r="I11" s="22">
         <v>205</v>
       </c>
-      <c r="J11" s="64" t="s">
+      <c r="J11" s="63" t="s">
         <v>127</v>
       </c>
       <c r="M11" s="4">
@@ -1639,7 +1663,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A12" s="4">
         <v>56</v>
       </c>
@@ -1667,7 +1691,7 @@
       <c r="I12" s="22">
         <v>205</v>
       </c>
-      <c r="J12" s="64" t="s">
+      <c r="J12" s="63" t="s">
         <v>128</v>
       </c>
       <c r="M12" s="4">
@@ -1683,7 +1707,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A13" s="4">
         <v>56</v>
       </c>
@@ -1711,7 +1735,7 @@
       <c r="I13" s="22">
         <v>205</v>
       </c>
-      <c r="J13" s="64" t="s">
+      <c r="J13" s="63" t="s">
         <v>126</v>
       </c>
       <c r="M13" s="4">
@@ -1727,7 +1751,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A14" s="4">
         <v>56</v>
       </c>
@@ -1755,7 +1779,7 @@
       <c r="I14" s="22">
         <v>205</v>
       </c>
-      <c r="J14" s="64" t="s">
+      <c r="J14" s="63" t="s">
         <v>124</v>
       </c>
       <c r="M14" s="4">
@@ -1771,7 +1795,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A15" s="7">
         <v>56</v>
       </c>
@@ -1787,7 +1811,7 @@
       <c r="E15" s="8">
         <v>6</v>
       </c>
-      <c r="F15" s="57" t="s">
+      <c r="F15" s="56" t="s">
         <v>37</v>
       </c>
       <c r="G15" s="9">
@@ -1796,10 +1820,10 @@
       <c r="H15" s="8">
         <v>3893</v>
       </c>
-      <c r="I15" s="56">
+      <c r="I15" s="55">
         <v>205</v>
       </c>
-      <c r="J15" s="66" t="s">
+      <c r="J15" s="65" t="s">
         <v>125</v>
       </c>
       <c r="M15" s="7">
@@ -1815,7 +1839,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A16" s="4">
         <v>57</v>
       </c>
@@ -1843,11 +1867,11 @@
       <c r="I16" s="22">
         <v>205</v>
       </c>
-      <c r="J16" s="64" t="s">
+      <c r="J16" s="63" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="4">
         <v>57</v>
       </c>
@@ -1875,14 +1899,14 @@
       <c r="I17" s="22">
         <v>205</v>
       </c>
-      <c r="J17" s="64" t="s">
+      <c r="J17" s="63" t="s">
         <v>122</v>
       </c>
       <c r="N17" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="4">
         <v>57</v>
       </c>
@@ -1910,11 +1934,11 @@
       <c r="I18" s="22">
         <v>205</v>
       </c>
-      <c r="J18" s="64" t="s">
+      <c r="J18" s="63" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="7">
         <v>57</v>
       </c>
@@ -1930,7 +1954,7 @@
       <c r="E19" s="8">
         <v>6</v>
       </c>
-      <c r="F19" s="57" t="s">
+      <c r="F19" s="56" t="s">
         <v>37</v>
       </c>
       <c r="G19" s="9">
@@ -1939,10 +1963,10 @@
       <c r="H19" s="8">
         <v>3893</v>
       </c>
-      <c r="I19" s="56">
+      <c r="I19" s="55">
         <v>205</v>
       </c>
-      <c r="J19" s="66" t="s">
+      <c r="J19" s="65" t="s">
         <v>120</v>
       </c>
       <c r="M19" s="15"/>
@@ -1954,7 +1978,7 @@
       <c r="Q19" s="3"/>
       <c r="R19" s="26"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
         <v>58</v>
       </c>
@@ -1982,7 +2006,7 @@
       <c r="I20" s="22">
         <v>205</v>
       </c>
-      <c r="J20" s="64" t="s">
+      <c r="J20" s="63" t="s">
         <v>116</v>
       </c>
       <c r="M20" s="12" t="s">
@@ -2013,7 +2037,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
         <v>58</v>
       </c>
@@ -2041,7 +2065,7 @@
       <c r="I21" s="22">
         <v>205</v>
       </c>
-      <c r="J21" s="64" t="s">
+      <c r="J21" s="63" t="s">
         <v>117</v>
       </c>
       <c r="M21" s="15">
@@ -2070,7 +2094,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="7">
         <v>58</v>
       </c>
@@ -2086,7 +2110,7 @@
       <c r="E22" s="8">
         <v>6</v>
       </c>
-      <c r="F22" s="58" t="s">
+      <c r="F22" s="57" t="s">
         <v>38</v>
       </c>
       <c r="G22" s="9">
@@ -2095,10 +2119,10 @@
       <c r="H22" s="8">
         <v>3799</v>
       </c>
-      <c r="I22" s="56">
+      <c r="I22" s="55">
         <v>205</v>
       </c>
-      <c r="J22" s="66" t="s">
+      <c r="J22" s="65" t="s">
         <v>118</v>
       </c>
       <c r="M22" s="4">
@@ -2130,7 +2154,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="4">
         <v>59</v>
       </c>
@@ -2158,7 +2182,7 @@
       <c r="I23" s="22">
         <v>196</v>
       </c>
-      <c r="J23" s="72" t="s">
+      <c r="J23" s="71" t="s">
         <v>77</v>
       </c>
       <c r="M23" s="4">
@@ -2190,7 +2214,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="4">
         <v>59</v>
       </c>
@@ -2218,7 +2242,7 @@
       <c r="I24" s="22">
         <v>205</v>
       </c>
-      <c r="J24" s="64" t="s">
+      <c r="J24" s="63" t="s">
         <v>78</v>
       </c>
       <c r="M24" s="4">
@@ -2250,7 +2274,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="7">
         <v>59</v>
       </c>
@@ -2275,10 +2299,10 @@
       <c r="H25" s="8">
         <v>3813</v>
       </c>
-      <c r="I25" s="56">
+      <c r="I25" s="55">
         <v>205</v>
       </c>
-      <c r="J25" s="66" t="s">
+      <c r="J25" s="65" t="s">
         <v>79</v>
       </c>
       <c r="M25" s="7">
@@ -2310,7 +2334,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="4">
         <v>60</v>
       </c>
@@ -2338,7 +2362,7 @@
       <c r="I26" s="22">
         <v>196</v>
       </c>
-      <c r="J26" s="64" t="s">
+      <c r="J26" s="63" t="s">
         <v>80</v>
       </c>
       <c r="K26" t="s">
@@ -2351,7 +2375,7 @@
       <c r="Q26" s="1"/>
       <c r="R26" s="31"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="4">
         <v>60</v>
       </c>
@@ -2379,7 +2403,7 @@
       <c r="I27" s="22">
         <v>196</v>
       </c>
-      <c r="J27" s="64" t="s">
+      <c r="J27" s="63" t="s">
         <v>81</v>
       </c>
       <c r="M27" s="1"/>
@@ -2389,7 +2413,7 @@
       <c r="Q27" s="1"/>
       <c r="R27" s="31"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="4">
         <v>60</v>
       </c>
@@ -2417,7 +2441,7 @@
       <c r="I28" s="22">
         <v>214</v>
       </c>
-      <c r="J28" s="64" t="s">
+      <c r="J28" s="63" t="s">
         <v>82</v>
       </c>
       <c r="M28" s="1"/>
@@ -2426,7 +2450,7 @@
       <c r="P28" s="1"/>
       <c r="Q28" s="1"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="7">
         <v>60</v>
       </c>
@@ -2442,7 +2466,7 @@
       <c r="E29" s="8">
         <v>3</v>
       </c>
-      <c r="F29" s="55" t="s">
+      <c r="F29" s="54" t="s">
         <v>54</v>
       </c>
       <c r="G29" s="9">
@@ -2451,10 +2475,10 @@
       <c r="H29" s="8">
         <v>3895</v>
       </c>
-      <c r="I29" s="56">
+      <c r="I29" s="55">
         <v>214</v>
       </c>
-      <c r="J29" s="66" t="s">
+      <c r="J29" s="65" t="s">
         <v>83</v>
       </c>
       <c r="M29" s="1"/>
@@ -2463,7 +2487,7 @@
       <c r="P29" s="1"/>
       <c r="Q29" s="1"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="4">
         <v>61</v>
       </c>
@@ -2491,7 +2515,7 @@
       <c r="I30" s="22">
         <v>196</v>
       </c>
-      <c r="J30" s="64" t="s">
+      <c r="J30" s="63" t="s">
         <v>84</v>
       </c>
       <c r="M30" s="1"/>
@@ -2500,7 +2524,7 @@
       <c r="P30" s="1"/>
       <c r="Q30" s="1"/>
     </row>
-    <row r="31" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A31" s="4">
         <v>61</v>
       </c>
@@ -2528,7 +2552,7 @@
       <c r="I31" s="22">
         <v>196</v>
       </c>
-      <c r="J31" s="64" t="s">
+      <c r="J31" s="63" t="s">
         <v>85</v>
       </c>
       <c r="M31" s="1"/>
@@ -2537,7 +2561,7 @@
       <c r="P31" s="1"/>
       <c r="Q31" s="1"/>
     </row>
-    <row r="32" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A32" s="4">
         <v>61</v>
       </c>
@@ -2565,7 +2589,7 @@
       <c r="I32" s="22">
         <v>214</v>
       </c>
-      <c r="J32" s="64" t="s">
+      <c r="J32" s="63" t="s">
         <v>86</v>
       </c>
       <c r="K32" t="s">
@@ -2578,7 +2602,7 @@
       <c r="Q32" s="1"/>
       <c r="R32" s="31"/>
     </row>
-    <row r="33" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A33" s="4">
         <v>61</v>
       </c>
@@ -2606,7 +2630,7 @@
       <c r="I33" s="22">
         <v>214</v>
       </c>
-      <c r="J33" s="64" t="s">
+      <c r="J33" s="63" t="s">
         <v>87</v>
       </c>
       <c r="M33" s="1"/>
@@ -2615,7 +2639,7 @@
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
     </row>
-    <row r="34" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A34" s="4">
         <v>61</v>
       </c>
@@ -2643,7 +2667,7 @@
       <c r="I34" s="22">
         <v>214</v>
       </c>
-      <c r="J34" s="64" t="s">
+      <c r="J34" s="63" t="s">
         <v>88</v>
       </c>
       <c r="M34" s="32" t="s">
@@ -2655,7 +2679,7 @@
       <c r="Q34" s="1"/>
       <c r="R34" s="31"/>
     </row>
-    <row r="35" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A35" s="7">
         <v>61</v>
       </c>
@@ -2671,7 +2695,7 @@
       <c r="E35" s="8">
         <v>3</v>
       </c>
-      <c r="F35" s="55" t="s">
+      <c r="F35" s="54" t="s">
         <v>54</v>
       </c>
       <c r="G35" s="9">
@@ -2680,10 +2704,10 @@
       <c r="H35" s="8">
         <v>3895</v>
       </c>
-      <c r="I35" s="56">
+      <c r="I35" s="55">
         <v>214</v>
       </c>
-      <c r="J35" s="66" t="s">
+      <c r="J35" s="65" t="s">
         <v>89</v>
       </c>
       <c r="M35" s="1"/>
@@ -2693,7 +2717,7 @@
       <c r="Q35" s="1"/>
       <c r="R35" s="31"/>
     </row>
-    <row r="36" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A36" s="4">
         <v>62</v>
       </c>
@@ -2721,16 +2745,16 @@
       <c r="I36" s="22">
         <v>214</v>
       </c>
-      <c r="J36" s="64" t="s">
+      <c r="J36" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="M36" s="74" t="s">
+      <c r="M36" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="N36" s="74"/>
-      <c r="O36" s="74"/>
-    </row>
-    <row r="37" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="N36" s="73"/>
+      <c r="O36" s="73"/>
+    </row>
+    <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
         <v>62</v>
       </c>
@@ -2758,11 +2782,11 @@
       <c r="I37" s="22">
         <v>214</v>
       </c>
-      <c r="J37" s="64" t="s">
+      <c r="J37" s="63" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="38" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A38" s="4">
         <v>62</v>
       </c>
@@ -2790,7 +2814,7 @@
       <c r="I38" s="22">
         <v>214</v>
       </c>
-      <c r="J38" s="64" t="s">
+      <c r="J38" s="63" t="s">
         <v>135</v>
       </c>
       <c r="M38" s="15"/>
@@ -2800,7 +2824,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="39" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A39" s="4">
         <v>62</v>
       </c>
@@ -2828,7 +2852,7 @@
       <c r="I39" s="22">
         <v>214</v>
       </c>
-      <c r="J39" s="64" t="s">
+      <c r="J39" s="63" t="s">
         <v>91</v>
       </c>
       <c r="M39" s="12" t="s">
@@ -2844,7 +2868,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="40" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A40" s="4">
         <v>62</v>
       </c>
@@ -2872,7 +2896,7 @@
       <c r="I40" s="22">
         <v>214</v>
       </c>
-      <c r="J40" s="64" t="s">
+      <c r="J40" s="63" t="s">
         <v>92</v>
       </c>
       <c r="M40" s="4">
@@ -2888,7 +2912,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="41" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A41" s="4">
         <v>62</v>
       </c>
@@ -2916,7 +2940,7 @@
       <c r="I41" s="22">
         <v>214</v>
       </c>
-      <c r="J41" s="64" t="s">
+      <c r="J41" s="63" t="s">
         <v>93</v>
       </c>
       <c r="M41" s="4">
@@ -2932,7 +2956,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="42" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A42" s="7">
         <v>62</v>
       </c>
@@ -2948,7 +2972,7 @@
       <c r="E42" s="8">
         <v>3</v>
       </c>
-      <c r="F42" s="55" t="s">
+      <c r="F42" s="54" t="s">
         <v>54</v>
       </c>
       <c r="G42" s="9">
@@ -2957,10 +2981,10 @@
       <c r="H42" s="8">
         <v>3895</v>
       </c>
-      <c r="I42" s="56">
+      <c r="I42" s="55">
         <v>214</v>
       </c>
-      <c r="J42" s="66" t="s">
+      <c r="J42" s="65" t="s">
         <v>94</v>
       </c>
       <c r="M42" s="33">
@@ -2976,7 +3000,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="43" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A43" s="4">
         <v>63</v>
       </c>
@@ -3004,7 +3028,7 @@
       <c r="I43" s="22">
         <v>214</v>
       </c>
-      <c r="J43" s="72" t="s">
+      <c r="J43" s="71" t="s">
         <v>99</v>
       </c>
       <c r="M43" s="37">
@@ -3020,7 +3044,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="44" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A44" s="4">
         <v>63</v>
       </c>
@@ -3048,11 +3072,11 @@
       <c r="I44" s="22">
         <v>214</v>
       </c>
-      <c r="J44" s="64" t="s">
+      <c r="J44" s="63" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="45" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A45" s="4">
         <v>63</v>
       </c>
@@ -3080,14 +3104,14 @@
       <c r="I45" s="22">
         <v>214</v>
       </c>
-      <c r="J45" s="64" t="s">
+      <c r="J45" s="63" t="s">
         <v>96</v>
       </c>
       <c r="N45" s="23" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="46" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A46" s="7">
         <v>63</v>
       </c>
@@ -3112,17 +3136,17 @@
       <c r="H46" s="8">
         <v>423</v>
       </c>
-      <c r="I46" s="56">
+      <c r="I46" s="55">
         <v>214</v>
       </c>
-      <c r="J46" s="71" t="s">
+      <c r="J46" s="70" t="s">
         <v>97</v>
       </c>
-      <c r="K46" s="70" t="s">
+      <c r="K46" s="69" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="47" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A47" s="4">
         <v>64</v>
       </c>
@@ -3150,7 +3174,7 @@
       <c r="I47" s="6">
         <v>240</v>
       </c>
-      <c r="J47" s="72" t="s">
+      <c r="J47" s="71" t="s">
         <v>98</v>
       </c>
       <c r="K47" t="s">
@@ -3165,7 +3189,7 @@
       <c r="Q47" s="3"/>
       <c r="R47" s="26"/>
     </row>
-    <row r="48" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A48" s="4">
         <v>64</v>
       </c>
@@ -3193,7 +3217,7 @@
       <c r="I48" s="6">
         <v>240</v>
       </c>
-      <c r="J48" s="72" t="s">
+      <c r="J48" s="71" t="s">
         <v>105</v>
       </c>
       <c r="M48" s="12" t="s">
@@ -3224,7 +3248,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="7">
         <v>64</v>
       </c>
@@ -3240,7 +3264,7 @@
       <c r="E49" s="8">
         <v>3</v>
       </c>
-      <c r="F49" s="55" t="s">
+      <c r="F49" s="54" t="s">
         <v>58</v>
       </c>
       <c r="G49" s="9">
@@ -3249,10 +3273,10 @@
       <c r="H49" s="8">
         <v>3895</v>
       </c>
-      <c r="I49" s="56">
+      <c r="I49" s="55">
         <v>214</v>
       </c>
-      <c r="J49" s="66" t="s">
+      <c r="J49" s="65" t="s">
         <v>112</v>
       </c>
       <c r="M49" s="15">
@@ -3281,7 +3305,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="4">
         <v>65</v>
       </c>
@@ -3309,7 +3333,7 @@
       <c r="I50" s="6">
         <v>235</v>
       </c>
-      <c r="J50" s="64" t="s">
+      <c r="J50" s="63" t="s">
         <v>111</v>
       </c>
       <c r="M50" s="4">
@@ -3338,7 +3362,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" s="4">
         <v>65</v>
       </c>
@@ -3366,7 +3390,7 @@
       <c r="I51" s="6">
         <v>235</v>
       </c>
-      <c r="J51" s="64" t="s">
+      <c r="J51" s="63" t="s">
         <v>106</v>
       </c>
       <c r="M51" s="4">
@@ -3395,7 +3419,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" s="7">
         <v>65</v>
       </c>
@@ -3411,7 +3435,7 @@
       <c r="E52" s="8">
         <v>6</v>
       </c>
-      <c r="F52" s="55" t="s">
+      <c r="F52" s="54" t="s">
         <v>76</v>
       </c>
       <c r="G52" s="9">
@@ -3423,7 +3447,7 @@
       <c r="I52" s="9">
         <v>235</v>
       </c>
-      <c r="J52" s="66" t="s">
+      <c r="J52" s="65" t="s">
         <v>107</v>
       </c>
       <c r="M52" s="4">
@@ -3452,7 +3476,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" s="4">
         <v>66</v>
       </c>
@@ -3480,7 +3504,7 @@
       <c r="I53" s="6">
         <v>235</v>
       </c>
-      <c r="J53" s="65" t="s">
+      <c r="J53" s="64" t="s">
         <v>110</v>
       </c>
       <c r="M53" s="37">
@@ -3509,7 +3533,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" s="4">
         <v>66</v>
       </c>
@@ -3537,11 +3561,11 @@
       <c r="I54" s="6">
         <v>235</v>
       </c>
-      <c r="J54" s="67" t="s">
+      <c r="J54" s="66" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" s="7">
         <v>66</v>
       </c>
@@ -3569,11 +3593,11 @@
       <c r="I55" s="9">
         <v>235</v>
       </c>
-      <c r="J55" s="68" t="s">
+      <c r="J55" s="67" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" s="15">
         <v>68</v>
       </c>
@@ -3601,11 +3625,11 @@
       <c r="I56" s="52">
         <v>235</v>
       </c>
-      <c r="J56" s="54" t="s">
+      <c r="J56" s="68" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="57" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" s="7">
         <v>68</v>
       </c>
@@ -3621,7 +3645,7 @@
       <c r="E57" s="8">
         <v>6</v>
       </c>
-      <c r="F57" s="55" t="s">
+      <c r="F57" s="54" t="s">
         <v>76</v>
       </c>
       <c r="G57" s="9">
@@ -3633,11 +3657,11 @@
       <c r="I57" s="9">
         <v>235</v>
       </c>
-      <c r="J57" s="50" t="s">
+      <c r="J57" s="65" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" s="4">
         <v>69</v>
       </c>
@@ -3665,11 +3689,11 @@
       <c r="I58" s="52">
         <v>235</v>
       </c>
-      <c r="J58" s="49" t="s">
+      <c r="J58" s="63" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" s="7">
         <v>69</v>
       </c>
@@ -3685,7 +3709,7 @@
       <c r="E59" s="8">
         <v>6</v>
       </c>
-      <c r="F59" s="55" t="s">
+      <c r="F59" s="54" t="s">
         <v>144</v>
       </c>
       <c r="G59" s="9">
@@ -3697,79 +3721,153 @@
       <c r="I59" s="9">
         <v>235</v>
       </c>
-      <c r="J59" s="50" t="s">
+      <c r="J59" s="65" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" s="4">
         <v>70</v>
       </c>
-      <c r="B60" s="1"/>
-      <c r="C60" s="1"/>
-      <c r="D60" s="4"/>
-      <c r="E60" s="1"/>
-      <c r="F60" s="1"/>
-      <c r="G60" s="6"/>
-      <c r="H60" s="1"/>
-      <c r="I60" s="6"/>
-      <c r="J60" s="49"/>
+      <c r="B60" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D60" s="4">
+        <v>60</v>
+      </c>
+      <c r="E60" s="1">
+        <v>6</v>
+      </c>
+      <c r="F60" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="G60" s="6">
+        <v>12</v>
+      </c>
+      <c r="H60" s="1">
+        <v>3928</v>
+      </c>
+      <c r="I60" s="52">
+        <v>235</v>
+      </c>
+      <c r="J60" s="49" t="s">
+        <v>152</v>
+      </c>
       <c r="M60" s="32" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="1"/>
-      <c r="C61" s="1"/>
-      <c r="D61" s="4"/>
-      <c r="E61" s="1"/>
-      <c r="F61" s="1"/>
-      <c r="G61" s="6"/>
-      <c r="H61" s="1"/>
-      <c r="I61" s="6"/>
-      <c r="J61" s="49"/>
-    </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A62" s="4"/>
-      <c r="B62" s="1"/>
-      <c r="C62" s="1"/>
-      <c r="D62" s="4"/>
-      <c r="E62" s="1"/>
-      <c r="F62" s="1"/>
-      <c r="G62" s="6"/>
-      <c r="H62" s="1"/>
-      <c r="I62" s="6"/>
-      <c r="J62" s="49"/>
-      <c r="N62" s="74" t="s">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A61" s="7">
+        <v>70</v>
+      </c>
+      <c r="B61" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C61" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D61" s="7">
+        <v>60</v>
+      </c>
+      <c r="E61" s="8">
         <v>6</v>
       </c>
-      <c r="O62" s="74"/>
-      <c r="P62" s="74"/>
-    </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A63" s="4"/>
-      <c r="B63" s="1"/>
-      <c r="C63" s="1"/>
+      <c r="F61" s="54" t="s">
+        <v>144</v>
+      </c>
+      <c r="G61" s="9">
+        <v>12</v>
+      </c>
+      <c r="H61" s="8">
+        <v>3936</v>
+      </c>
+      <c r="I61" s="9">
+        <v>235</v>
+      </c>
+      <c r="J61" s="50" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A62" s="77">
+        <v>71</v>
+      </c>
+      <c r="B62" s="78" t="s">
+        <v>5</v>
+      </c>
+      <c r="C62" s="78" t="s">
+        <v>73</v>
+      </c>
+      <c r="D62" s="77">
+        <v>60</v>
+      </c>
+      <c r="E62" s="78">
+        <v>6</v>
+      </c>
+      <c r="F62" s="78" t="s">
+        <v>143</v>
+      </c>
+      <c r="G62" s="79">
+        <v>12</v>
+      </c>
+      <c r="H62" s="78">
+        <v>3928</v>
+      </c>
+      <c r="I62" s="79">
+        <v>235</v>
+      </c>
+      <c r="J62" s="80" t="s">
+        <v>151</v>
+      </c>
+      <c r="N62" s="73" t="s">
+        <v>6</v>
+      </c>
+      <c r="O62" s="73"/>
+      <c r="P62" s="73"/>
+    </row>
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A63" s="4">
+        <v>72</v>
+      </c>
+      <c r="B63" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>73</v>
+      </c>
       <c r="D63" s="4"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="6"/>
       <c r="H63" s="1"/>
       <c r="I63" s="6"/>
-      <c r="J63" s="49"/>
-    </row>
-    <row r="64" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A64" s="4"/>
-      <c r="B64" s="1"/>
-      <c r="C64" s="1"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="1"/>
-      <c r="F64" s="1"/>
-      <c r="G64" s="6"/>
-      <c r="H64" s="1"/>
-      <c r="I64" s="6"/>
-      <c r="J64" s="49"/>
+      <c r="J63" s="49" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A64" s="7">
+        <v>72</v>
+      </c>
+      <c r="B64" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="C64" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="D64" s="7"/>
+      <c r="E64" s="8"/>
+      <c r="F64" s="8"/>
+      <c r="G64" s="9"/>
+      <c r="H64" s="8"/>
+      <c r="I64" s="9"/>
+      <c r="J64" s="50" t="s">
+        <v>150</v>
+      </c>
       <c r="M64" s="15"/>
       <c r="N64" s="16"/>
       <c r="O64" s="16"/>
@@ -3777,7 +3875,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A65" s="4"/>
       <c r="B65" s="1"/>
       <c r="C65" s="1"/>
@@ -3801,7 +3899,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A66" s="4"/>
       <c r="B66" s="1"/>
       <c r="C66" s="1"/>
@@ -3825,7 +3923,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A67" s="4"/>
       <c r="B67" s="1"/>
       <c r="C67" s="1"/>
@@ -3849,7 +3947,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A68" s="7"/>
       <c r="B68" s="8"/>
       <c r="C68" s="8"/>
@@ -3873,7 +3971,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A69" s="1"/>
       <c r="B69" s="1"/>
       <c r="C69" s="1"/>
@@ -3896,7 +3994,7 @@
         <v>235</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A70" s="1"/>
       <c r="B70" s="1"/>
       <c r="C70" s="1"/>
@@ -3910,7 +4008,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A71" s="1"/>
       <c r="B71" s="1"/>
       <c r="C71" s="1"/>
@@ -3921,7 +4019,7 @@
       <c r="H71" s="1"/>
       <c r="I71" s="1"/>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:22" x14ac:dyDescent="0.3">
       <c r="M72" s="15"/>
       <c r="N72" s="16"/>
       <c r="O72" s="16"/>
@@ -3931,7 +4029,7 @@
       <c r="Q72" s="3"/>
       <c r="R72" s="26"/>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:22" x14ac:dyDescent="0.3">
       <c r="M73" s="12" t="s">
         <v>7</v>
       </c>
@@ -3960,7 +4058,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:22" x14ac:dyDescent="0.3">
       <c r="M74" s="15">
         <v>15</v>
       </c>
@@ -3990,7 +4088,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:22" x14ac:dyDescent="0.3">
       <c r="M75" s="1">
         <v>15</v>
       </c>
@@ -4017,7 +4115,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:22" x14ac:dyDescent="0.3">
       <c r="M76" s="41">
         <v>15</v>
       </c>
@@ -4044,11 +4142,11 @@
         <v>63</v>
       </c>
     </row>
-    <row r="81" spans="13:22" x14ac:dyDescent="0.25">
-      <c r="M81" s="62"/>
+    <row r="81" spans="13:22" x14ac:dyDescent="0.3">
+      <c r="M81" s="61"/>
       <c r="N81" s="10"/>
       <c r="O81" s="10"/>
-      <c r="P81" s="63" t="s">
+      <c r="P81" s="62" t="s">
         <v>66</v>
       </c>
       <c r="Q81" s="10" t="s">
@@ -4056,8 +4154,8 @@
       </c>
       <c r="R81" s="11"/>
     </row>
-    <row r="82" spans="13:22" x14ac:dyDescent="0.25">
-      <c r="M82" s="59">
+    <row r="82" spans="13:22" x14ac:dyDescent="0.3">
+      <c r="M82" s="58">
         <v>60</v>
       </c>
       <c r="N82">
@@ -4086,8 +4184,8 @@
         <v>72</v>
       </c>
     </row>
-    <row r="83" spans="13:22" x14ac:dyDescent="0.25">
-      <c r="M83" s="59">
+    <row r="83" spans="13:22" x14ac:dyDescent="0.3">
+      <c r="M83" s="58">
         <v>60</v>
       </c>
       <c r="N83">
@@ -4116,8 +4214,8 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="13:22" x14ac:dyDescent="0.25">
-      <c r="M84" s="59">
+    <row r="84" spans="13:22" x14ac:dyDescent="0.3">
+      <c r="M84" s="58">
         <v>60</v>
       </c>
       <c r="N84">
@@ -4143,8 +4241,8 @@
         <v>74</v>
       </c>
     </row>
-    <row r="85" spans="13:22" x14ac:dyDescent="0.25">
-      <c r="M85" s="59">
+    <row r="85" spans="13:22" x14ac:dyDescent="0.3">
+      <c r="M85" s="58">
         <v>60</v>
       </c>
       <c r="N85">
@@ -4170,20 +4268,20 @@
         <v>101</v>
       </c>
     </row>
-    <row r="86" spans="13:22" x14ac:dyDescent="0.25">
-      <c r="M86" s="60">
+    <row r="86" spans="13:22" x14ac:dyDescent="0.3">
+      <c r="M86" s="59">
         <v>60</v>
       </c>
-      <c r="N86" s="58">
+      <c r="N86" s="57">
         <v>6</v>
       </c>
-      <c r="O86" s="58">
+      <c r="O86" s="57">
         <v>12</v>
       </c>
-      <c r="P86" s="61">
+      <c r="P86" s="60">
         <v>3914</v>
       </c>
-      <c r="Q86" s="58">
+      <c r="Q86" s="57">
         <v>235</v>
       </c>
       <c r="R86" s="29" t="s">
@@ -4197,7 +4295,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="88" spans="13:22" x14ac:dyDescent="0.25">
+    <row r="88" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M88">
         <v>60</v>
       </c>
@@ -4224,7 +4322,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="89" spans="13:22" x14ac:dyDescent="0.25">
+    <row r="89" spans="13:22" x14ac:dyDescent="0.3">
       <c r="M89">
         <v>60</v>
       </c>
@@ -4260,7 +4358,7 @@
     <mergeCell ref="N62:P62"/>
   </mergeCells>
   <conditionalFormatting sqref="H5">
-    <cfRule type="iconSet" priority="101">
+    <cfRule type="iconSet" priority="104">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4268,7 +4366,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="102">
+    <cfRule type="iconSet" priority="105">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4278,7 +4376,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5">
-    <cfRule type="colorScale" priority="98">
+    <cfRule type="colorScale" priority="101">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4286,7 +4384,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="100">
+    <cfRule type="colorScale" priority="103">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4298,7 +4396,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6:J9">
-    <cfRule type="colorScale" priority="62">
+    <cfRule type="colorScale" priority="65">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4306,7 +4404,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="63">
+    <cfRule type="colorScale" priority="66">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4318,7 +4416,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H6:H30 H32:H35">
-    <cfRule type="iconSet" priority="60">
+    <cfRule type="iconSet" priority="63">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4326,7 +4424,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="61">
+    <cfRule type="iconSet" priority="64">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4336,7 +4434,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H31">
-    <cfRule type="iconSet" priority="56">
+    <cfRule type="iconSet" priority="59">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4344,7 +4442,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="57">
+    <cfRule type="iconSet" priority="60">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4354,7 +4452,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10:J22 I24:J35 I23 J16:J31">
-    <cfRule type="colorScale" priority="54">
+    <cfRule type="colorScale" priority="57">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4362,7 +4460,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="55">
+    <cfRule type="colorScale" priority="58">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4374,7 +4472,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J22 I47:J48 I24:J35 I23 J16:J31 I50:J52 I53:I54">
-    <cfRule type="colorScale" priority="52">
+    <cfRule type="colorScale" priority="55">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4386,7 +4484,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H36:H37">
-    <cfRule type="iconSet" priority="50">
+    <cfRule type="iconSet" priority="53">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4394,7 +4492,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="51">
+    <cfRule type="iconSet" priority="54">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4404,7 +4502,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:J37">
-    <cfRule type="colorScale" priority="48">
+    <cfRule type="colorScale" priority="51">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4412,7 +4510,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="49">
+    <cfRule type="colorScale" priority="52">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4424,7 +4522,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I36:J37">
-    <cfRule type="colorScale" priority="47">
+    <cfRule type="colorScale" priority="50">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4436,7 +4534,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H38:H39">
-    <cfRule type="iconSet" priority="45">
+    <cfRule type="iconSet" priority="48">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4444,7 +4542,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="46">
+    <cfRule type="iconSet" priority="49">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4454,7 +4552,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:J39">
-    <cfRule type="colorScale" priority="43">
+    <cfRule type="colorScale" priority="46">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4462,7 +4560,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="44">
+    <cfRule type="colorScale" priority="47">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4474,7 +4572,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:J39">
-    <cfRule type="colorScale" priority="42">
+    <cfRule type="colorScale" priority="45">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4486,7 +4584,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H40">
-    <cfRule type="iconSet" priority="40">
+    <cfRule type="iconSet" priority="43">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4494,7 +4592,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="41">
+    <cfRule type="iconSet" priority="44">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4504,7 +4602,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:J40">
-    <cfRule type="colorScale" priority="38">
+    <cfRule type="colorScale" priority="41">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4512,7 +4610,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="39">
+    <cfRule type="colorScale" priority="42">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4524,7 +4622,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:J40">
-    <cfRule type="colorScale" priority="37">
+    <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4536,7 +4634,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H41:H42">
-    <cfRule type="iconSet" priority="35">
+    <cfRule type="iconSet" priority="38">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4544,7 +4642,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="36">
+    <cfRule type="iconSet" priority="39">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4554,7 +4652,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:J42">
-    <cfRule type="colorScale" priority="33">
+    <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4562,7 +4660,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="34">
+    <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4574,7 +4672,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:J42">
-    <cfRule type="colorScale" priority="32">
+    <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4586,7 +4684,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H43">
-    <cfRule type="iconSet" priority="30">
+    <cfRule type="iconSet" priority="33">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4594,7 +4692,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="31">
+    <cfRule type="iconSet" priority="34">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4604,7 +4702,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:J43">
-    <cfRule type="colorScale" priority="28">
+    <cfRule type="colorScale" priority="31">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4612,7 +4710,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="29">
+    <cfRule type="colorScale" priority="32">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4624,7 +4722,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I43:J43">
-    <cfRule type="colorScale" priority="27">
+    <cfRule type="colorScale" priority="30">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4636,7 +4734,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H44">
-    <cfRule type="iconSet" priority="25">
+    <cfRule type="iconSet" priority="28">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4644,7 +4742,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="26">
+    <cfRule type="iconSet" priority="29">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4654,7 +4752,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44:J44">
-    <cfRule type="colorScale" priority="23">
+    <cfRule type="colorScale" priority="26">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4662,7 +4760,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="24">
+    <cfRule type="colorScale" priority="27">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4674,7 +4772,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I44:J44">
-    <cfRule type="colorScale" priority="22">
+    <cfRule type="colorScale" priority="25">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4686,7 +4784,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H45">
-    <cfRule type="iconSet" priority="20">
+    <cfRule type="iconSet" priority="23">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4694,7 +4792,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="21">
+    <cfRule type="iconSet" priority="24">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4704,7 +4802,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:J45">
-    <cfRule type="colorScale" priority="18">
+    <cfRule type="colorScale" priority="21">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4712,7 +4810,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="19">
+    <cfRule type="colorScale" priority="22">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4724,7 +4822,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I45:J45">
-    <cfRule type="colorScale" priority="17">
+    <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4736,7 +4834,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H46">
-    <cfRule type="iconSet" priority="15">
+    <cfRule type="iconSet" priority="18">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4744,7 +4842,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="16">
+    <cfRule type="iconSet" priority="19">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4754,7 +4852,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46:J46">
-    <cfRule type="colorScale" priority="13">
+    <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4762,7 +4860,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="14">
+    <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4774,7 +4872,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I46:J46">
-    <cfRule type="colorScale" priority="12">
+    <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4786,7 +4884,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="H49">
-    <cfRule type="iconSet" priority="10">
+    <cfRule type="iconSet" priority="13">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="num" val="500"/>
@@ -4794,7 +4892,7 @@
         <cfvo type="num" val="3850"/>
       </iconSet>
     </cfRule>
-    <cfRule type="iconSet" priority="11">
+    <cfRule type="iconSet" priority="14">
       <iconSet iconSet="4TrafficLights">
         <cfvo type="percent" val="0"/>
         <cfvo type="percent" val="25"/>
@@ -4804,7 +4902,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:J49">
-    <cfRule type="colorScale" priority="8">
+    <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="max"/>
@@ -4812,7 +4910,7 @@
         <color rgb="FF63BE7B"/>
       </colorScale>
     </cfRule>
-    <cfRule type="colorScale" priority="9">
+    <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4824,6 +4922,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I49:J49">
+    <cfRule type="colorScale" priority="10">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I55">
+    <cfRule type="colorScale" priority="9">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I56">
+    <cfRule type="colorScale" priority="8">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I57">
     <cfRule type="colorScale" priority="7">
       <colorScale>
         <cfvo type="min"/>
@@ -4835,7 +4969,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I55">
+  <conditionalFormatting sqref="I58">
     <cfRule type="colorScale" priority="6">
       <colorScale>
         <cfvo type="min"/>
@@ -4847,19 +4981,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I56">
-    <cfRule type="colorScale" priority="5">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I57">
+  <conditionalFormatting sqref="I59">
     <cfRule type="colorScale" priority="4">
       <colorScale>
         <cfvo type="min"/>
@@ -4871,7 +4993,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I58">
+  <conditionalFormatting sqref="I60">
     <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="min"/>
@@ -4883,7 +5005,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I59">
+  <conditionalFormatting sqref="I61">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I62">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>

<commit_message>
Phobos xslx updated; special pointings LTP planning with 5 obs per STP
</commit_message>
<xml_diff>
--- a/observations/phobos_deimos/phobos_deimos.xlsx
+++ b/observations/phobos_deimos/phobos_deimos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\phobos_deimos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89D40F26-5DCF-4E81-A4DD-97714BE3154F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA779192-FF6F-4D4C-9A4F-7B91D60F16D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -480,13 +480,13 @@
     <t>2023-10-27T08:30:15</t>
   </si>
   <si>
-    <t>2023-09-03T02:37:30</t>
-  </si>
-  <si>
-    <t>2023-08-28T01:12:00</t>
-  </si>
-  <si>
-    <t>2023-08-30T06:15:30</t>
+    <t>20230828_010044</t>
+  </si>
+  <si>
+    <t>20230830_060414</t>
+  </si>
+  <si>
+    <t>20230903_022613</t>
   </si>
 </sst>
 </file>
@@ -957,9 +957,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -971,6 +968,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="15" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1257,8 +1257,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="H69" sqref="H69"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1281,16 +1281,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="M1" s="77" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
+      <c r="B1" s="76"/>
+      <c r="C1" s="76"/>
+      <c r="M1" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="76"/>
+      <c r="O1" s="76"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J2" s="72" t="s">
@@ -1301,12 +1301,12 @@
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="78" t="s">
+      <c r="D3" s="77" t="s">
         <v>12</v>
       </c>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="80"/>
+      <c r="E3" s="78"/>
+      <c r="F3" s="78"/>
+      <c r="G3" s="79"/>
       <c r="H3" s="10"/>
       <c r="I3" s="11"/>
       <c r="J3" s="72" t="s">
@@ -2748,11 +2748,11 @@
       <c r="J36" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="M36" s="77" t="s">
-        <v>6</v>
-      </c>
-      <c r="N36" s="77"/>
-      <c r="O36" s="77"/>
+      <c r="M36" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="N36" s="76"/>
+      <c r="O36" s="76"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
@@ -3753,8 +3753,8 @@
       <c r="I60" s="52">
         <v>235</v>
       </c>
-      <c r="J60" s="49" t="s">
-        <v>152</v>
+      <c r="J60" s="63" t="s">
+        <v>151</v>
       </c>
       <c r="M60" s="32" t="s">
         <v>55</v>
@@ -3788,8 +3788,8 @@
       <c r="I61" s="9">
         <v>235</v>
       </c>
-      <c r="J61" s="50" t="s">
-        <v>153</v>
+      <c r="J61" s="65" t="s">
+        <v>152</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
@@ -3820,14 +3820,14 @@
       <c r="I62" s="75">
         <v>235</v>
       </c>
-      <c r="J62" s="76" t="s">
-        <v>151</v>
-      </c>
-      <c r="N62" s="77" t="s">
-        <v>6</v>
-      </c>
-      <c r="O62" s="77"/>
-      <c r="P62" s="77"/>
+      <c r="J62" s="80" t="s">
+        <v>153</v>
+      </c>
+      <c r="N62" s="76" t="s">
+        <v>6</v>
+      </c>
+      <c r="O62" s="76"/>
+      <c r="P62" s="76"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="4">

</xml_diff>

<commit_message>
Phobos deimos obs list updated
</commit_message>
<xml_diff>
--- a/observations/phobos_deimos/phobos_deimos.xlsx
+++ b/observations/phobos_deimos/phobos_deimos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\phobos_deimos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A13F29-C0F4-42BC-AAD8-28A26C4E690C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6DD013C-46C0-465A-A6B0-952D72F5287F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="41496" windowHeight="16776" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -474,12 +474,6 @@
     <t>20230703_193210</t>
   </si>
   <si>
-    <t>2023-10-24T11:43:30</t>
-  </si>
-  <si>
-    <t>2023-10-27T08:30:15</t>
-  </si>
-  <si>
     <t>20230828_010044</t>
   </si>
   <si>
@@ -501,9 +495,6 @@
     <t>2024-01-14T17:42:00</t>
   </si>
   <si>
-    <t>2023-12-14T12:59:00</t>
-  </si>
-  <si>
     <t>2023-12-20T14:24:30</t>
   </si>
   <si>
@@ -514,6 +505,15 @@
   </si>
   <si>
     <t>2024-02-15T17:04:00</t>
+  </si>
+  <si>
+    <t>20231024_113219</t>
+  </si>
+  <si>
+    <t>20231027_081904</t>
+  </si>
+  <si>
+    <t>20231214_124745</t>
   </si>
 </sst>
 </file>
@@ -793,7 +793,7 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="82">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1000,9 +1000,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1290,8 +1287,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="A75" sqref="A75"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F63" sqref="F63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3787,7 +3784,7 @@
         <v>235</v>
       </c>
       <c r="J60" s="63" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M60" s="32" t="s">
         <v>55</v>
@@ -3822,7 +3819,7 @@
         <v>235</v>
       </c>
       <c r="J61" s="65" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:21" x14ac:dyDescent="0.3">
@@ -3854,7 +3851,7 @@
         <v>235</v>
       </c>
       <c r="J62" s="76" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="N62" s="78" t="s">
         <v>6</v>
@@ -3891,7 +3888,7 @@
         <v>235</v>
       </c>
       <c r="J63" s="49" t="s">
-        <v>149</v>
+        <v>160</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.3">
@@ -3923,7 +3920,7 @@
         <v>235</v>
       </c>
       <c r="J64" s="50" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="M64" s="15"/>
       <c r="N64" s="16"/>
@@ -3961,7 +3958,7 @@
         <v>235</v>
       </c>
       <c r="J65" s="49" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="M65" s="12" t="s">
         <v>7</v>
@@ -4005,7 +4002,7 @@
         <v>235</v>
       </c>
       <c r="J66" s="50" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="M66" s="41">
         <v>15</v>
@@ -4049,7 +4046,7 @@
         <v>235</v>
       </c>
       <c r="J67" s="77" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="M67">
         <v>30</v>
@@ -4093,7 +4090,7 @@
         <v>235</v>
       </c>
       <c r="J68" s="49" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M68">
         <v>60</v>
@@ -4137,7 +4134,7 @@
         <v>235</v>
       </c>
       <c r="J69" s="49" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="M69">
         <v>60</v>
@@ -4181,7 +4178,7 @@
         <v>235</v>
       </c>
       <c r="J70" s="50" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="N70" s="23" t="s">
         <v>23</v>
@@ -4216,7 +4213,7 @@
         <v>235</v>
       </c>
       <c r="J71" s="49" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="72" spans="1:22" x14ac:dyDescent="0.3">
@@ -4248,7 +4245,7 @@
         <v>235</v>
       </c>
       <c r="J72" s="49" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="M72" s="15"/>
       <c r="N72" s="16"/>
@@ -4288,7 +4285,7 @@
         <v>235</v>
       </c>
       <c r="J73" s="50" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="M73" s="12" t="s">
         <v>7</v>
@@ -4319,7 +4316,7 @@
       </c>
     </row>
     <row r="74" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A74" s="82">
+      <c r="A74" s="1">
         <v>77</v>
       </c>
       <c r="M74" s="15">

</xml_diff>

<commit_message>
New FTP checker code draft working locally
</commit_message>
<xml_diff>
--- a/observations/phobos_deimos/phobos_deimos.xlsx
+++ b/observations/phobos_deimos/phobos_deimos.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\iant\Documents\PROGRAMS\nomad_obs\observations\phobos_deimos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35321E8B-2C77-4D66-A807-057B8E808868}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BBC9622-D5BE-4DE6-83E8-79079EDE8889}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="466" uniqueCount="180">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="468" uniqueCount="183">
   <si>
     <t>PHOBOS DEIMOS COP ROWS</t>
   </si>
@@ -576,6 +576,15 @@
   </si>
   <si>
     <t>2024-06-06T01:38:08</t>
+  </si>
+  <si>
+    <t>3770,3794,3808,3828,0,0 # ORDERS 163 165 167 169 -- NADIR_12ROWS_60SECS_4SUBDS -- EXECTIME=59492MS</t>
+  </si>
+  <si>
+    <t>Hydration band 2: 163, 165, 167, 169 500ms</t>
+  </si>
+  <si>
+    <t>HYDRATION BAND#2 163 165 167 169</t>
   </si>
 </sst>
 </file>
@@ -1078,33 +1087,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Bad" xfId="1" builtinId="27"/>
@@ -1388,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V90"/>
+  <dimension ref="A1:V91"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="A93" sqref="A93"/>
+    <sheetView tabSelected="1" topLeftCell="A66" workbookViewId="0">
+      <selection activeCell="F86" sqref="F86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1414,16 +1417,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="89" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="M1" s="86" t="s">
-        <v>6</v>
-      </c>
-      <c r="N1" s="86"/>
-      <c r="O1" s="86"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="M1" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="N1" s="89"/>
+      <c r="O1" s="89"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.3">
       <c r="J2" s="72" t="s">
@@ -1434,12 +1437,12 @@
       <c r="A3" s="2"/>
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
-      <c r="D3" s="87" t="s">
-        <v>12</v>
-      </c>
-      <c r="E3" s="88"/>
-      <c r="F3" s="88"/>
-      <c r="G3" s="89"/>
+      <c r="D3" s="90" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="91"/>
+      <c r="F3" s="91"/>
+      <c r="G3" s="92"/>
       <c r="H3" s="10"/>
       <c r="I3" s="11"/>
       <c r="J3" s="72" t="s">
@@ -2881,11 +2884,11 @@
       <c r="J36" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="M36" s="86" t="s">
-        <v>6</v>
-      </c>
-      <c r="N36" s="86"/>
-      <c r="O36" s="86"/>
+      <c r="M36" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="N36" s="89"/>
+      <c r="O36" s="89"/>
     </row>
     <row r="37" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A37" s="4">
@@ -3956,11 +3959,11 @@
       <c r="J62" s="76" t="s">
         <v>151</v>
       </c>
-      <c r="N62" s="86" t="s">
-        <v>6</v>
-      </c>
-      <c r="O62" s="86"/>
-      <c r="P62" s="86"/>
+      <c r="N62" s="89" t="s">
+        <v>6</v>
+      </c>
+      <c r="O62" s="89"/>
+      <c r="P62" s="89"/>
     </row>
     <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" s="4">
@@ -4910,7 +4913,7 @@
       <c r="I84" s="16">
         <v>235</v>
       </c>
-      <c r="J84" s="94" t="s">
+      <c r="J84" s="86" t="s">
         <v>178</v>
       </c>
       <c r="M84" s="58">
@@ -4967,7 +4970,7 @@
       <c r="I85" s="8">
         <v>235</v>
       </c>
-      <c r="J85" s="95" t="s">
+      <c r="J85" s="87" t="s">
         <v>179</v>
       </c>
       <c r="M85" s="58">
@@ -4997,7 +5000,7 @@
       </c>
     </row>
     <row r="86" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A86" s="90">
+      <c r="A86" s="15">
         <v>81</v>
       </c>
       <c r="B86" s="16" t="s">
@@ -5010,21 +5013,21 @@
         <v>60</v>
       </c>
       <c r="E86" s="16">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F86" s="16" t="s">
-        <v>143</v>
+        <v>182</v>
       </c>
       <c r="G86" s="52">
         <v>12</v>
       </c>
       <c r="H86" s="16">
-        <v>3928</v>
+        <v>3951</v>
       </c>
       <c r="I86" s="52">
         <v>235</v>
       </c>
-      <c r="J86" s="94" t="s">
+      <c r="J86" s="86" t="s">
         <v>174</v>
       </c>
       <c r="M86" s="59">
@@ -5054,84 +5057,90 @@
       </c>
     </row>
     <row r="87" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A87" s="91">
+      <c r="A87" s="4">
         <v>81</v>
       </c>
-      <c r="B87" s="92" t="s">
-        <v>5</v>
-      </c>
-      <c r="C87" s="92" t="s">
+      <c r="B87" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C87" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D87" s="4">
         <v>60</v>
       </c>
-      <c r="E87" s="92">
-        <v>6</v>
-      </c>
-      <c r="F87" s="92" t="s">
-        <v>144</v>
+      <c r="E87" s="1">
+        <v>4</v>
+      </c>
+      <c r="F87" s="93" t="s">
+        <v>182</v>
       </c>
       <c r="G87" s="6">
         <v>12</v>
       </c>
-      <c r="H87" s="92">
-        <v>3936</v>
+      <c r="H87" s="1">
+        <v>3951</v>
       </c>
       <c r="I87" s="6">
         <v>235</v>
       </c>
-      <c r="J87" s="96" t="s">
+      <c r="J87" s="88" t="s">
         <v>175</v>
       </c>
+      <c r="M87" s="2"/>
+      <c r="N87" s="3"/>
+      <c r="O87" s="3"/>
+      <c r="P87" s="3"/>
+      <c r="Q87" s="3"/>
+      <c r="R87" s="26"/>
     </row>
     <row r="88" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A88" s="91">
+      <c r="A88" s="4">
         <v>81</v>
       </c>
-      <c r="B88" s="92" t="s">
-        <v>5</v>
-      </c>
-      <c r="C88" s="92" t="s">
+      <c r="B88" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C88" s="1" t="s">
         <v>73</v>
       </c>
       <c r="D88" s="4">
         <v>60</v>
       </c>
-      <c r="E88" s="92">
-        <v>6</v>
-      </c>
-      <c r="F88" s="92" t="s">
-        <v>143</v>
+      <c r="E88" s="1">
+        <v>4</v>
+      </c>
+      <c r="F88" s="93" t="s">
+        <v>182</v>
       </c>
       <c r="G88" s="6">
         <v>12</v>
       </c>
-      <c r="H88" s="92">
-        <v>3928</v>
+      <c r="H88" s="1">
+        <v>3951</v>
       </c>
       <c r="I88" s="6">
         <v>235</v>
       </c>
-      <c r="J88" s="96" t="s">
+      <c r="J88" s="88" t="s">
         <v>176</v>
       </c>
-      <c r="M88">
+      <c r="M88" s="58">
         <v>60</v>
       </c>
-      <c r="N88">
-        <v>6</v>
-      </c>
-      <c r="O88">
-        <v>12</v>
-      </c>
-      <c r="P88" s="23">
+      <c r="N88" s="94">
+        <v>6</v>
+      </c>
+      <c r="O88" s="94">
+        <v>12</v>
+      </c>
+      <c r="P88" s="95">
         <v>3928</v>
       </c>
-      <c r="Q88">
+      <c r="Q88" s="94">
         <v>235</v>
       </c>
-      <c r="R88" t="s">
+      <c r="R88" s="27" t="s">
         <v>142</v>
       </c>
       <c r="T88">
@@ -5143,7 +5152,7 @@
       </c>
     </row>
     <row r="89" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A89" s="93">
+      <c r="A89" s="7">
         <v>81</v>
       </c>
       <c r="B89" s="8" t="s">
@@ -5156,43 +5165,43 @@
         <v>60</v>
       </c>
       <c r="E89" s="8">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F89" s="8" t="s">
-        <v>144</v>
+        <v>182</v>
       </c>
       <c r="G89" s="9">
         <v>12</v>
       </c>
       <c r="H89" s="8">
-        <v>3936</v>
+        <v>3951</v>
       </c>
       <c r="I89" s="9">
         <v>235</v>
       </c>
-      <c r="J89" s="95" t="s">
+      <c r="J89" s="87" t="s">
         <v>177</v>
       </c>
-      <c r="M89">
+      <c r="M89" s="58">
         <v>60</v>
       </c>
-      <c r="N89">
-        <v>6</v>
-      </c>
-      <c r="O89">
-        <v>12</v>
-      </c>
-      <c r="P89" s="23">
+      <c r="N89" s="94">
+        <v>6</v>
+      </c>
+      <c r="O89" s="94">
+        <v>12</v>
+      </c>
+      <c r="P89" s="95">
         <v>3936</v>
       </c>
-      <c r="Q89">
+      <c r="Q89" s="94">
         <v>235</v>
       </c>
-      <c r="R89" t="s">
+      <c r="R89" s="27" t="s">
         <v>141</v>
       </c>
       <c r="T89">
-        <f t="shared" ref="T89" si="1">P89+2</f>
+        <f t="shared" ref="T89:T91" si="1">P89+2</f>
         <v>3938</v>
       </c>
       <c r="U89" t="s">
@@ -5200,8 +5209,41 @@
       </c>
     </row>
     <row r="90" spans="1:22" x14ac:dyDescent="0.3">
-      <c r="A90" s="91">
+      <c r="A90" s="4">
         <v>82</v>
+      </c>
+      <c r="M90" s="58"/>
+      <c r="N90" s="94"/>
+      <c r="O90" s="94"/>
+      <c r="P90" s="94"/>
+      <c r="Q90" s="94"/>
+      <c r="R90" s="27"/>
+    </row>
+    <row r="91" spans="1:22" x14ac:dyDescent="0.3">
+      <c r="M91" s="59">
+        <v>60</v>
+      </c>
+      <c r="N91" s="57">
+        <v>4</v>
+      </c>
+      <c r="O91" s="57">
+        <v>12</v>
+      </c>
+      <c r="P91" s="60">
+        <v>3951</v>
+      </c>
+      <c r="Q91" s="57">
+        <v>235</v>
+      </c>
+      <c r="R91" s="96" t="s">
+        <v>181</v>
+      </c>
+      <c r="T91">
+        <f t="shared" si="1"/>
+        <v>3953</v>
+      </c>
+      <c r="U91" t="s">
+        <v>180</v>
       </c>
     </row>
   </sheetData>

</xml_diff>